<commit_message>
results of cat baseline added
</commit_message>
<xml_diff>
--- a/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
+++ b/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
@@ -5,18 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Github\Fani-Lab\lady\main\output\2015SB12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farinam\PycharmProjects\LADy\output\2015SB12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C72EF-4129-4DBF-93A5-DD5A7174E8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604B6812-30DD-4FBB-8AD7-605BE20B00D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="96">
   <si>
     <t>metric</t>
   </si>
@@ -303,6 +308,30 @@
   <si>
     <t>semeval-15-restaurant</t>
   </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>arabic.cat</t>
+  </si>
+  <si>
+    <t>german.cat</t>
+  </si>
+  <si>
+    <t>french.cat</t>
+  </si>
+  <si>
+    <t>farsi.cat</t>
+  </si>
+  <si>
+    <t>chinese.cat</t>
+  </si>
+  <si>
+    <t>spanish.cat</t>
+  </si>
+  <si>
+    <t>all.cat</t>
+  </si>
 </sst>
 </file>
 
@@ -311,7 +340,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +364,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -344,7 +378,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -383,11 +417,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -409,11 +458,14 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,6 +651,1147 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>metric</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>cat.0.0</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>arb_Arab.cat.0.0</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>deu_Latn.cat.0.0</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>fra_Latn.cat.0.0</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>pes_Arab.cat.0.0</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>zho_Hans.cat.0.0</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>spa_Latn.cat.0.0</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>pes_Arab.zho_Hans.deu_Latn.arb_Arab.fra_Latn.spa_Latn.cat.0.0</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>P_1</v>
+          </cell>
+          <cell r="B2">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="C2">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="D2">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="E2">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="F2">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="G2">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="H2">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="I2">
+            <v>0.598019801980198</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>P_5</v>
+          </cell>
+          <cell r="B3">
+            <v>0.10495049504950479</v>
+          </cell>
+          <cell r="C3">
+            <v>0.1136633663366335</v>
+          </cell>
+          <cell r="D3">
+            <v>0.11009900990099</v>
+          </cell>
+          <cell r="E3">
+            <v>0.1116831683168316</v>
+          </cell>
+          <cell r="F3">
+            <v>0.1077227722772276</v>
+          </cell>
+          <cell r="G3">
+            <v>0.1057425742574256</v>
+          </cell>
+          <cell r="H3">
+            <v>0.1132673267326731</v>
+          </cell>
+          <cell r="I3">
+            <v>0.1572277227722769</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>P_10</v>
+          </cell>
+          <cell r="B4">
+            <v>6.07920792079207E-2</v>
+          </cell>
+          <cell r="C4">
+            <v>6.3168316831683002E-2</v>
+          </cell>
+          <cell r="D4">
+            <v>6.0198019801980099E-2</v>
+          </cell>
+          <cell r="E4">
+            <v>6.2970297029702901E-2</v>
+          </cell>
+          <cell r="F4">
+            <v>5.9801980198019702E-2</v>
+          </cell>
+          <cell r="G4">
+            <v>5.8811881188118698E-2</v>
+          </cell>
+          <cell r="H4">
+            <v>6.0198019801980099E-2</v>
+          </cell>
+          <cell r="I4">
+            <v>7.9801980198019595E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>P_100</v>
+          </cell>
+          <cell r="B5">
+            <v>8.0990099009900993E-3</v>
+          </cell>
+          <cell r="C5">
+            <v>8.2178217821782008E-3</v>
+          </cell>
+          <cell r="D5">
+            <v>8.0198019801979992E-3</v>
+          </cell>
+          <cell r="E5">
+            <v>8.1782178217821005E-3</v>
+          </cell>
+          <cell r="F5">
+            <v>8.0594059405940006E-3</v>
+          </cell>
+          <cell r="G5">
+            <v>7.9603960396038998E-3</v>
+          </cell>
+          <cell r="H5">
+            <v>8.1584158415840997E-3</v>
+          </cell>
+          <cell r="I5">
+            <v>8.1782178217821005E-3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>recall_1</v>
+          </cell>
+          <cell r="B6">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="C6">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="D6">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="E6">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="F6">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="G6">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="H6">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="I6">
+            <v>0.598019801980198</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>recall_5</v>
+          </cell>
+          <cell r="B7">
+            <v>0.52475247524752477</v>
+          </cell>
+          <cell r="C7">
+            <v>0.56831683168316827</v>
+          </cell>
+          <cell r="D7">
+            <v>0.55049504950495054</v>
+          </cell>
+          <cell r="E7">
+            <v>0.55841584158415847</v>
+          </cell>
+          <cell r="F7">
+            <v>0.53861386138613865</v>
+          </cell>
+          <cell r="G7">
+            <v>0.52871287128712874</v>
+          </cell>
+          <cell r="H7">
+            <v>0.56633663366336628</v>
+          </cell>
+          <cell r="I7">
+            <v>0.78613861386138617</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>recall_10</v>
+          </cell>
+          <cell r="B8">
+            <v>0.60792079207920791</v>
+          </cell>
+          <cell r="C8">
+            <v>0.63168316831683169</v>
+          </cell>
+          <cell r="D8">
+            <v>0.60198019801980196</v>
+          </cell>
+          <cell r="E8">
+            <v>0.62970297029702971</v>
+          </cell>
+          <cell r="F8">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="G8">
+            <v>0.58811881188118809</v>
+          </cell>
+          <cell r="H8">
+            <v>0.60198019801980196</v>
+          </cell>
+          <cell r="I8">
+            <v>0.79801980198019806</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>recall_100</v>
+          </cell>
+          <cell r="B9">
+            <v>0.80990099009900995</v>
+          </cell>
+          <cell r="C9">
+            <v>0.82178217821782185</v>
+          </cell>
+          <cell r="D9">
+            <v>0.80198019801980203</v>
+          </cell>
+          <cell r="E9">
+            <v>0.81782178217821788</v>
+          </cell>
+          <cell r="F9">
+            <v>0.80594059405940599</v>
+          </cell>
+          <cell r="G9">
+            <v>0.79603960396039608</v>
+          </cell>
+          <cell r="H9">
+            <v>0.8158415841584159</v>
+          </cell>
+          <cell r="I9">
+            <v>0.81782178217821788</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>ndcg_cut_1</v>
+          </cell>
+          <cell r="B10">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="C10">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="D10">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="E10">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="F10">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="G10">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="H10">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="I10">
+            <v>0.598019801980198</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>ndcg_cut_5</v>
+          </cell>
+          <cell r="B11">
+            <v>0.43433685881132428</v>
+          </cell>
+          <cell r="C11">
+            <v>0.49393158719216779</v>
+          </cell>
+          <cell r="D11">
+            <v>0.47867078650248568</v>
+          </cell>
+          <cell r="E11">
+            <v>0.48832212190279489</v>
+          </cell>
+          <cell r="F11">
+            <v>0.45923120656909389</v>
+          </cell>
+          <cell r="G11">
+            <v>0.45956591316347828</v>
+          </cell>
+          <cell r="H11">
+            <v>0.4841750282211964</v>
+          </cell>
+          <cell r="I11">
+            <v>0.70960729180542281</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>ndcg_cut_10</v>
+          </cell>
+          <cell r="B12">
+            <v>0.46142184532764291</v>
+          </cell>
+          <cell r="C12">
+            <v>0.51453621143316575</v>
+          </cell>
+          <cell r="D12">
+            <v>0.49479441345825409</v>
+          </cell>
+          <cell r="E12">
+            <v>0.51124006193511495</v>
+          </cell>
+          <cell r="F12">
+            <v>0.47881210170055832</v>
+          </cell>
+          <cell r="G12">
+            <v>0.479215482410146</v>
+          </cell>
+          <cell r="H12">
+            <v>0.49566258216036968</v>
+          </cell>
+          <cell r="I12">
+            <v>0.71358751120038144</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>ndcg_cut_100</v>
+          </cell>
+          <cell r="B13">
+            <v>0.50529935513018653</v>
+          </cell>
+          <cell r="C13">
+            <v>0.55670661377860775</v>
+          </cell>
+          <cell r="D13">
+            <v>0.53687811583328249</v>
+          </cell>
+          <cell r="E13">
+            <v>0.55128375161457255</v>
+          </cell>
+          <cell r="F13">
+            <v>0.52282318292622265</v>
+          </cell>
+          <cell r="G13">
+            <v>0.52150583498395298</v>
+          </cell>
+          <cell r="H13">
+            <v>0.54132733999753324</v>
+          </cell>
+          <cell r="I13">
+            <v>0.71728765166300479</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>map_cut_1</v>
+          </cell>
+          <cell r="B14">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="C14">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="D14">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="E14">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="F14">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="G14">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="H14">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="I14">
+            <v>0.598019801980198</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>map_cut_5</v>
+          </cell>
+          <cell r="B15">
+            <v>0.40422442244224421</v>
+          </cell>
+          <cell r="C15">
+            <v>0.46937293729372931</v>
+          </cell>
+          <cell r="D15">
+            <v>0.45485148514851481</v>
+          </cell>
+          <cell r="E15">
+            <v>0.46478547854785479</v>
+          </cell>
+          <cell r="F15">
+            <v>0.43280528052805273</v>
+          </cell>
+          <cell r="G15">
+            <v>0.43623762376237629</v>
+          </cell>
+          <cell r="H15">
+            <v>0.45689768976897688</v>
+          </cell>
+          <cell r="I15">
+            <v>0.68306930693069312</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>map_cut_10</v>
+          </cell>
+          <cell r="B16">
+            <v>0.4155209806694955</v>
+          </cell>
+          <cell r="C16">
+            <v>0.47794593745088798</v>
+          </cell>
+          <cell r="D16">
+            <v>0.46118890460474621</v>
+          </cell>
+          <cell r="E16">
+            <v>0.47417256011315417</v>
+          </cell>
+          <cell r="F16">
+            <v>0.44110639635392113</v>
+          </cell>
+          <cell r="G16">
+            <v>0.44461260411755471</v>
+          </cell>
+          <cell r="H16">
+            <v>0.46161873330190162</v>
+          </cell>
+          <cell r="I16">
+            <v>0.68479019330504476</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>map_cut_100</v>
+          </cell>
+          <cell r="B17">
+            <v>0.42488362742894498</v>
+          </cell>
+          <cell r="C17">
+            <v>0.4872134221457734</v>
+          </cell>
+          <cell r="D17">
+            <v>0.469563637924027</v>
+          </cell>
+          <cell r="E17">
+            <v>0.4822241441449609</v>
+          </cell>
+          <cell r="F17">
+            <v>0.4498824784876414</v>
+          </cell>
+          <cell r="G17">
+            <v>0.45234578405123521</v>
+          </cell>
+          <cell r="H17">
+            <v>0.47104781340409702</v>
+          </cell>
+          <cell r="I17">
+            <v>0.68536277648194477</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>success_1</v>
+          </cell>
+          <cell r="B18">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="C18">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="D18">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="E18">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="F18">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="G18">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="H18">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="I18">
+            <v>0.598019801980198</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>success_5</v>
+          </cell>
+          <cell r="B19">
+            <v>0.52475247524752477</v>
+          </cell>
+          <cell r="C19">
+            <v>0.56831683168316827</v>
+          </cell>
+          <cell r="D19">
+            <v>0.55049504950495054</v>
+          </cell>
+          <cell r="E19">
+            <v>0.55841584158415847</v>
+          </cell>
+          <cell r="F19">
+            <v>0.53861386138613865</v>
+          </cell>
+          <cell r="G19">
+            <v>0.52871287128712874</v>
+          </cell>
+          <cell r="H19">
+            <v>0.56633663366336628</v>
+          </cell>
+          <cell r="I19">
+            <v>0.78613861386138617</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>success_10</v>
+          </cell>
+          <cell r="B20">
+            <v>0.60792079207920791</v>
+          </cell>
+          <cell r="C20">
+            <v>0.63168316831683169</v>
+          </cell>
+          <cell r="D20">
+            <v>0.60198019801980196</v>
+          </cell>
+          <cell r="E20">
+            <v>0.62970297029702971</v>
+          </cell>
+          <cell r="F20">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="G20">
+            <v>0.58811881188118809</v>
+          </cell>
+          <cell r="H20">
+            <v>0.60198019801980196</v>
+          </cell>
+          <cell r="I20">
+            <v>0.79801980198019806</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>success_100</v>
+          </cell>
+          <cell r="B21">
+            <v>0.80990099009900995</v>
+          </cell>
+          <cell r="C21">
+            <v>0.82178217821782185</v>
+          </cell>
+          <cell r="D21">
+            <v>0.80198019801980203</v>
+          </cell>
+          <cell r="E21">
+            <v>0.81782178217821788</v>
+          </cell>
+          <cell r="F21">
+            <v>0.80594059405940599</v>
+          </cell>
+          <cell r="G21">
+            <v>0.79603960396039608</v>
+          </cell>
+          <cell r="H21">
+            <v>0.8158415841584159</v>
+          </cell>
+          <cell r="I21">
+            <v>0.81782178217821788</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>metric</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>P_1</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>P_5</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>P_10</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>recall_1</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>recall_5</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>recall_10</v>
+          </cell>
+          <cell r="J1" t="str">
+            <v>ndcg_cut_1</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>ndcg_cut_5</v>
+          </cell>
+          <cell r="L1" t="str">
+            <v>ndcg_cut_10</v>
+          </cell>
+          <cell r="N1" t="str">
+            <v>map_cut_1</v>
+          </cell>
+          <cell r="O1" t="str">
+            <v>map_cut_5</v>
+          </cell>
+          <cell r="P1" t="str">
+            <v>map_cut_10</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>cat</v>
+          </cell>
+          <cell r="B2">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="C2">
+            <v>0.10495049504950479</v>
+          </cell>
+          <cell r="D2">
+            <v>6.07920792079207E-2</v>
+          </cell>
+          <cell r="F2">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="G2">
+            <v>0.52475247524752477</v>
+          </cell>
+          <cell r="H2">
+            <v>0.60792079207920791</v>
+          </cell>
+          <cell r="J2">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="K2">
+            <v>0.43433685881132428</v>
+          </cell>
+          <cell r="L2">
+            <v>0.46142184532764291</v>
+          </cell>
+          <cell r="N2">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="O2">
+            <v>0.40422442244224421</v>
+          </cell>
+          <cell r="P2">
+            <v>0.4155209806694955</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>arabic.cat</v>
+          </cell>
+          <cell r="B3">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="C3">
+            <v>0.1136633663366335</v>
+          </cell>
+          <cell r="D3">
+            <v>6.3168316831683002E-2</v>
+          </cell>
+          <cell r="F3">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="G3">
+            <v>0.56831683168316827</v>
+          </cell>
+          <cell r="H3">
+            <v>0.63168316831683169</v>
+          </cell>
+          <cell r="J3">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="K3">
+            <v>0.49393158719216779</v>
+          </cell>
+          <cell r="L3">
+            <v>0.51453621143316575</v>
+          </cell>
+          <cell r="N3">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="O3">
+            <v>0.46937293729372931</v>
+          </cell>
+          <cell r="P3">
+            <v>0.47794593745088798</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>german.cat</v>
+          </cell>
+          <cell r="B4">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="C4">
+            <v>0.11009900990099</v>
+          </cell>
+          <cell r="D4">
+            <v>6.0198019801980099E-2</v>
+          </cell>
+          <cell r="F4">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="G4">
+            <v>0.55049504950495054</v>
+          </cell>
+          <cell r="H4">
+            <v>0.60198019801980196</v>
+          </cell>
+          <cell r="J4">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="K4">
+            <v>0.47867078650248568</v>
+          </cell>
+          <cell r="L4">
+            <v>0.49479441345825409</v>
+          </cell>
+          <cell r="N4">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="O4">
+            <v>0.45485148514851481</v>
+          </cell>
+          <cell r="P4">
+            <v>0.46118890460474621</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>french.cat</v>
+          </cell>
+          <cell r="B5">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="C5">
+            <v>0.1116831683168316</v>
+          </cell>
+          <cell r="D5">
+            <v>6.2970297029702901E-2</v>
+          </cell>
+          <cell r="F5">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="G5">
+            <v>0.55841584158415847</v>
+          </cell>
+          <cell r="H5">
+            <v>0.62970297029702971</v>
+          </cell>
+          <cell r="J5">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="K5">
+            <v>0.48832212190279489</v>
+          </cell>
+          <cell r="L5">
+            <v>0.51124006193511495</v>
+          </cell>
+          <cell r="N5">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="O5">
+            <v>0.46478547854785479</v>
+          </cell>
+          <cell r="P5">
+            <v>0.47417256011315417</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>farsi.cat</v>
+          </cell>
+          <cell r="B6">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="C6">
+            <v>0.1077227722772276</v>
+          </cell>
+          <cell r="D6">
+            <v>5.9801980198019702E-2</v>
+          </cell>
+          <cell r="F6">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="G6">
+            <v>0.53861386138613865</v>
+          </cell>
+          <cell r="H6">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="J6">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="K6">
+            <v>0.45923120656909389</v>
+          </cell>
+          <cell r="L6">
+            <v>0.47881210170055832</v>
+          </cell>
+          <cell r="N6">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="O6">
+            <v>0.43280528052805273</v>
+          </cell>
+          <cell r="P6">
+            <v>0.44110639635392113</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>chinese.cat</v>
+          </cell>
+          <cell r="B7">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="C7">
+            <v>0.1057425742574256</v>
+          </cell>
+          <cell r="D7">
+            <v>5.8811881188118698E-2</v>
+          </cell>
+          <cell r="F7">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="G7">
+            <v>0.52871287128712874</v>
+          </cell>
+          <cell r="H7">
+            <v>0.58811881188118809</v>
+          </cell>
+          <cell r="J7">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="K7">
+            <v>0.45956591316347828</v>
+          </cell>
+          <cell r="L7">
+            <v>0.479215482410146</v>
+          </cell>
+          <cell r="N7">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="O7">
+            <v>0.43623762376237629</v>
+          </cell>
+          <cell r="P7">
+            <v>0.44461260411755471</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>spanish.cat</v>
+          </cell>
+          <cell r="B8">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="C8">
+            <v>0.1132673267326731</v>
+          </cell>
+          <cell r="D8">
+            <v>6.0198019801980099E-2</v>
+          </cell>
+          <cell r="F8">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="G8">
+            <v>0.56633663366336628</v>
+          </cell>
+          <cell r="H8">
+            <v>0.60198019801980196</v>
+          </cell>
+          <cell r="J8">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="K8">
+            <v>0.4841750282211964</v>
+          </cell>
+          <cell r="L8">
+            <v>0.49566258216036968</v>
+          </cell>
+          <cell r="N8">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="O8">
+            <v>0.45689768976897688</v>
+          </cell>
+          <cell r="P8">
+            <v>0.46161873330190162</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>all.cat</v>
+          </cell>
+          <cell r="B9">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="C9">
+            <v>0.1572277227722769</v>
+          </cell>
+          <cell r="D9">
+            <v>7.9801980198019595E-2</v>
+          </cell>
+          <cell r="F9">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="G9">
+            <v>0.78613861386138617</v>
+          </cell>
+          <cell r="H9">
+            <v>0.79801980198019806</v>
+          </cell>
+          <cell r="J9">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="K9">
+            <v>0.70960729180542281</v>
+          </cell>
+          <cell r="L9">
+            <v>0.71358751120038144</v>
+          </cell>
+          <cell r="N9">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="O9">
+            <v>0.68306930693069312</v>
+          </cell>
+          <cell r="P9">
+            <v>0.68479019330504476</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>0.33267326732673269</v>
+          </cell>
+          <cell r="C2">
+            <v>0.52475247524752477</v>
+          </cell>
+          <cell r="D2">
+            <v>0.43433685881132428</v>
+          </cell>
+          <cell r="E2">
+            <v>0.40422442244224421</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>0.37227722772277227</v>
+          </cell>
+          <cell r="C3">
+            <v>0.52871287128712874</v>
+          </cell>
+          <cell r="D3">
+            <v>0.45956591316347828</v>
+          </cell>
+          <cell r="E3">
+            <v>0.43623762376237629</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>0.37029702970297029</v>
+          </cell>
+          <cell r="C4">
+            <v>0.53861386138613865</v>
+          </cell>
+          <cell r="D4">
+            <v>0.45923120656909389</v>
+          </cell>
+          <cell r="E4">
+            <v>0.43280528052805273</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>0.4138613861386139</v>
+          </cell>
+          <cell r="C5">
+            <v>0.56831683168316827</v>
+          </cell>
+          <cell r="D5">
+            <v>0.49393158719216779</v>
+          </cell>
+          <cell r="E5">
+            <v>0.46937293729372931</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0.40396039603960399</v>
+          </cell>
+          <cell r="C6">
+            <v>0.55841584158415847</v>
+          </cell>
+          <cell r="D6">
+            <v>0.48832212190279489</v>
+          </cell>
+          <cell r="E6">
+            <v>0.46478547854785479</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>0.39801980198019798</v>
+          </cell>
+          <cell r="C7">
+            <v>0.55049504950495054</v>
+          </cell>
+          <cell r="D7">
+            <v>0.47867078650248568</v>
+          </cell>
+          <cell r="E7">
+            <v>0.45485148514851481</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>0.39207920792079209</v>
+          </cell>
+          <cell r="C8">
+            <v>0.56633663366336628</v>
+          </cell>
+          <cell r="D8">
+            <v>0.4841750282211964</v>
+          </cell>
+          <cell r="E8">
+            <v>0.45689768976897688</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>0.598019801980198</v>
+          </cell>
+          <cell r="C9">
+            <v>0.78613861386138617</v>
+          </cell>
+          <cell r="D9">
+            <v>0.70960729180542281</v>
+          </cell>
+          <cell r="E9">
+            <v>0.68306930693069312</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -898,10 +2091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DE02BE-45B7-4D8D-BCA0-35520325FAF3}">
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I112" sqref="I112:I131"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4563,6 +5756,804 @@
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" t="str">
+        <f>[1]Sheet1!A1</f>
+        <v>metric</v>
+      </c>
+      <c r="B133" t="str">
+        <f>[1]Sheet1!B1</f>
+        <v>cat.0.0</v>
+      </c>
+      <c r="C133" t="str">
+        <f>[1]Sheet1!C1</f>
+        <v>arb_Arab.cat.0.0</v>
+      </c>
+      <c r="D133" t="str">
+        <f>[1]Sheet1!D1</f>
+        <v>deu_Latn.cat.0.0</v>
+      </c>
+      <c r="E133" t="str">
+        <f>[1]Sheet1!E1</f>
+        <v>fra_Latn.cat.0.0</v>
+      </c>
+      <c r="F133" t="str">
+        <f>[1]Sheet1!F1</f>
+        <v>pes_Arab.cat.0.0</v>
+      </c>
+      <c r="G133" t="str">
+        <f>[1]Sheet1!G1</f>
+        <v>zho_Hans.cat.0.0</v>
+      </c>
+      <c r="H133" t="str">
+        <f>[1]Sheet1!H1</f>
+        <v>spa_Latn.cat.0.0</v>
+      </c>
+      <c r="I133" t="str">
+        <f>[1]Sheet1!I1</f>
+        <v>pes_Arab.zho_Hans.deu_Latn.arb_Arab.fra_Latn.spa_Latn.cat.0.0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" t="str">
+        <f>[1]Sheet1!A2</f>
+        <v>P_1</v>
+      </c>
+      <c r="B134">
+        <f>[1]Sheet1!B2</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C134">
+        <f>[1]Sheet1!C2</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D134">
+        <f>[1]Sheet1!D2</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E134">
+        <f>[1]Sheet1!E2</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F134">
+        <f>[1]Sheet1!F2</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G134">
+        <f>[1]Sheet1!G2</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H134">
+        <f>[1]Sheet1!H2</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I134">
+        <f>[1]Sheet1!I2</f>
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="str">
+        <f>[1]Sheet1!A3</f>
+        <v>P_5</v>
+      </c>
+      <c r="B135">
+        <f>[1]Sheet1!B3</f>
+        <v>0.10495049504950479</v>
+      </c>
+      <c r="C135">
+        <f>[1]Sheet1!C3</f>
+        <v>0.1136633663366335</v>
+      </c>
+      <c r="D135">
+        <f>[1]Sheet1!D3</f>
+        <v>0.11009900990099</v>
+      </c>
+      <c r="E135">
+        <f>[1]Sheet1!E3</f>
+        <v>0.1116831683168316</v>
+      </c>
+      <c r="F135">
+        <f>[1]Sheet1!F3</f>
+        <v>0.1077227722772276</v>
+      </c>
+      <c r="G135">
+        <f>[1]Sheet1!G3</f>
+        <v>0.1057425742574256</v>
+      </c>
+      <c r="H135">
+        <f>[1]Sheet1!H3</f>
+        <v>0.1132673267326731</v>
+      </c>
+      <c r="I135">
+        <f>[1]Sheet1!I3</f>
+        <v>0.1572277227722769</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" t="str">
+        <f>[1]Sheet1!A4</f>
+        <v>P_10</v>
+      </c>
+      <c r="B136">
+        <f>[1]Sheet1!B4</f>
+        <v>6.07920792079207E-2</v>
+      </c>
+      <c r="C136">
+        <f>[1]Sheet1!C4</f>
+        <v>6.3168316831683002E-2</v>
+      </c>
+      <c r="D136">
+        <f>[1]Sheet1!D4</f>
+        <v>6.0198019801980099E-2</v>
+      </c>
+      <c r="E136">
+        <f>[1]Sheet1!E4</f>
+        <v>6.2970297029702901E-2</v>
+      </c>
+      <c r="F136">
+        <f>[1]Sheet1!F4</f>
+        <v>5.9801980198019702E-2</v>
+      </c>
+      <c r="G136">
+        <f>[1]Sheet1!G4</f>
+        <v>5.8811881188118698E-2</v>
+      </c>
+      <c r="H136">
+        <f>[1]Sheet1!H4</f>
+        <v>6.0198019801980099E-2</v>
+      </c>
+      <c r="I136">
+        <f>[1]Sheet1!I4</f>
+        <v>7.9801980198019595E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" t="str">
+        <f>[1]Sheet1!A5</f>
+        <v>P_100</v>
+      </c>
+      <c r="B137">
+        <f>[1]Sheet1!B5</f>
+        <v>8.0990099009900993E-3</v>
+      </c>
+      <c r="C137">
+        <f>[1]Sheet1!C5</f>
+        <v>8.2178217821782008E-3</v>
+      </c>
+      <c r="D137">
+        <f>[1]Sheet1!D5</f>
+        <v>8.0198019801979992E-3</v>
+      </c>
+      <c r="E137">
+        <f>[1]Sheet1!E5</f>
+        <v>8.1782178217821005E-3</v>
+      </c>
+      <c r="F137">
+        <f>[1]Sheet1!F5</f>
+        <v>8.0594059405940006E-3</v>
+      </c>
+      <c r="G137">
+        <f>[1]Sheet1!G5</f>
+        <v>7.9603960396038998E-3</v>
+      </c>
+      <c r="H137">
+        <f>[1]Sheet1!H5</f>
+        <v>8.1584158415840997E-3</v>
+      </c>
+      <c r="I137">
+        <f>[1]Sheet1!I5</f>
+        <v>8.1782178217821005E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="str">
+        <f>[1]Sheet1!A6</f>
+        <v>recall_1</v>
+      </c>
+      <c r="B138">
+        <f>[1]Sheet1!B6</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C138">
+        <f>[1]Sheet1!C6</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D138">
+        <f>[1]Sheet1!D6</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E138">
+        <f>[1]Sheet1!E6</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F138">
+        <f>[1]Sheet1!F6</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G138">
+        <f>[1]Sheet1!G6</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H138">
+        <f>[1]Sheet1!H6</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I138">
+        <f>[1]Sheet1!I6</f>
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" t="str">
+        <f>[1]Sheet1!A7</f>
+        <v>recall_5</v>
+      </c>
+      <c r="B139">
+        <f>[1]Sheet1!B7</f>
+        <v>0.52475247524752477</v>
+      </c>
+      <c r="C139">
+        <f>[1]Sheet1!C7</f>
+        <v>0.56831683168316827</v>
+      </c>
+      <c r="D139">
+        <f>[1]Sheet1!D7</f>
+        <v>0.55049504950495054</v>
+      </c>
+      <c r="E139">
+        <f>[1]Sheet1!E7</f>
+        <v>0.55841584158415847</v>
+      </c>
+      <c r="F139">
+        <f>[1]Sheet1!F7</f>
+        <v>0.53861386138613865</v>
+      </c>
+      <c r="G139">
+        <f>[1]Sheet1!G7</f>
+        <v>0.52871287128712874</v>
+      </c>
+      <c r="H139">
+        <f>[1]Sheet1!H7</f>
+        <v>0.56633663366336628</v>
+      </c>
+      <c r="I139">
+        <f>[1]Sheet1!I7</f>
+        <v>0.78613861386138617</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" t="str">
+        <f>[1]Sheet1!A8</f>
+        <v>recall_10</v>
+      </c>
+      <c r="B140">
+        <f>[1]Sheet1!B8</f>
+        <v>0.60792079207920791</v>
+      </c>
+      <c r="C140">
+        <f>[1]Sheet1!C8</f>
+        <v>0.63168316831683169</v>
+      </c>
+      <c r="D140">
+        <f>[1]Sheet1!D8</f>
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="E140">
+        <f>[1]Sheet1!E8</f>
+        <v>0.62970297029702971</v>
+      </c>
+      <c r="F140">
+        <f>[1]Sheet1!F8</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="G140">
+        <f>[1]Sheet1!G8</f>
+        <v>0.58811881188118809</v>
+      </c>
+      <c r="H140">
+        <f>[1]Sheet1!H8</f>
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="I140">
+        <f>[1]Sheet1!I8</f>
+        <v>0.79801980198019806</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" t="str">
+        <f>[1]Sheet1!A9</f>
+        <v>recall_100</v>
+      </c>
+      <c r="B141">
+        <f>[1]Sheet1!B9</f>
+        <v>0.80990099009900995</v>
+      </c>
+      <c r="C141">
+        <f>[1]Sheet1!C9</f>
+        <v>0.82178217821782185</v>
+      </c>
+      <c r="D141">
+        <f>[1]Sheet1!D9</f>
+        <v>0.80198019801980203</v>
+      </c>
+      <c r="E141">
+        <f>[1]Sheet1!E9</f>
+        <v>0.81782178217821788</v>
+      </c>
+      <c r="F141">
+        <f>[1]Sheet1!F9</f>
+        <v>0.80594059405940599</v>
+      </c>
+      <c r="G141">
+        <f>[1]Sheet1!G9</f>
+        <v>0.79603960396039608</v>
+      </c>
+      <c r="H141">
+        <f>[1]Sheet1!H9</f>
+        <v>0.8158415841584159</v>
+      </c>
+      <c r="I141">
+        <f>[1]Sheet1!I9</f>
+        <v>0.81782178217821788</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" t="str">
+        <f>[1]Sheet1!A10</f>
+        <v>ndcg_cut_1</v>
+      </c>
+      <c r="B142">
+        <f>[1]Sheet1!B10</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C142">
+        <f>[1]Sheet1!C10</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D142">
+        <f>[1]Sheet1!D10</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E142">
+        <f>[1]Sheet1!E10</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F142">
+        <f>[1]Sheet1!F10</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G142">
+        <f>[1]Sheet1!G10</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H142">
+        <f>[1]Sheet1!H10</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I142">
+        <f>[1]Sheet1!I10</f>
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="str">
+        <f>[1]Sheet1!A11</f>
+        <v>ndcg_cut_5</v>
+      </c>
+      <c r="B143">
+        <f>[1]Sheet1!B11</f>
+        <v>0.43433685881132428</v>
+      </c>
+      <c r="C143">
+        <f>[1]Sheet1!C11</f>
+        <v>0.49393158719216779</v>
+      </c>
+      <c r="D143">
+        <f>[1]Sheet1!D11</f>
+        <v>0.47867078650248568</v>
+      </c>
+      <c r="E143">
+        <f>[1]Sheet1!E11</f>
+        <v>0.48832212190279489</v>
+      </c>
+      <c r="F143">
+        <f>[1]Sheet1!F11</f>
+        <v>0.45923120656909389</v>
+      </c>
+      <c r="G143">
+        <f>[1]Sheet1!G11</f>
+        <v>0.45956591316347828</v>
+      </c>
+      <c r="H143">
+        <f>[1]Sheet1!H11</f>
+        <v>0.4841750282211964</v>
+      </c>
+      <c r="I143">
+        <f>[1]Sheet1!I11</f>
+        <v>0.70960729180542281</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" t="str">
+        <f>[1]Sheet1!A12</f>
+        <v>ndcg_cut_10</v>
+      </c>
+      <c r="B144">
+        <f>[1]Sheet1!B12</f>
+        <v>0.46142184532764291</v>
+      </c>
+      <c r="C144">
+        <f>[1]Sheet1!C12</f>
+        <v>0.51453621143316575</v>
+      </c>
+      <c r="D144">
+        <f>[1]Sheet1!D12</f>
+        <v>0.49479441345825409</v>
+      </c>
+      <c r="E144">
+        <f>[1]Sheet1!E12</f>
+        <v>0.51124006193511495</v>
+      </c>
+      <c r="F144">
+        <f>[1]Sheet1!F12</f>
+        <v>0.47881210170055832</v>
+      </c>
+      <c r="G144">
+        <f>[1]Sheet1!G12</f>
+        <v>0.479215482410146</v>
+      </c>
+      <c r="H144">
+        <f>[1]Sheet1!H12</f>
+        <v>0.49566258216036968</v>
+      </c>
+      <c r="I144">
+        <f>[1]Sheet1!I12</f>
+        <v>0.71358751120038144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" t="str">
+        <f>[1]Sheet1!A13</f>
+        <v>ndcg_cut_100</v>
+      </c>
+      <c r="B145">
+        <f>[1]Sheet1!B13</f>
+        <v>0.50529935513018653</v>
+      </c>
+      <c r="C145">
+        <f>[1]Sheet1!C13</f>
+        <v>0.55670661377860775</v>
+      </c>
+      <c r="D145">
+        <f>[1]Sheet1!D13</f>
+        <v>0.53687811583328249</v>
+      </c>
+      <c r="E145">
+        <f>[1]Sheet1!E13</f>
+        <v>0.55128375161457255</v>
+      </c>
+      <c r="F145">
+        <f>[1]Sheet1!F13</f>
+        <v>0.52282318292622265</v>
+      </c>
+      <c r="G145">
+        <f>[1]Sheet1!G13</f>
+        <v>0.52150583498395298</v>
+      </c>
+      <c r="H145">
+        <f>[1]Sheet1!H13</f>
+        <v>0.54132733999753324</v>
+      </c>
+      <c r="I145">
+        <f>[1]Sheet1!I13</f>
+        <v>0.71728765166300479</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" t="str">
+        <f>[1]Sheet1!A14</f>
+        <v>map_cut_1</v>
+      </c>
+      <c r="B146">
+        <f>[1]Sheet1!B14</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C146">
+        <f>[1]Sheet1!C14</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D146">
+        <f>[1]Sheet1!D14</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E146">
+        <f>[1]Sheet1!E14</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F146">
+        <f>[1]Sheet1!F14</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G146">
+        <f>[1]Sheet1!G14</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H146">
+        <f>[1]Sheet1!H14</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I146">
+        <f>[1]Sheet1!I14</f>
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" t="str">
+        <f>[1]Sheet1!A15</f>
+        <v>map_cut_5</v>
+      </c>
+      <c r="B147">
+        <f>[1]Sheet1!B15</f>
+        <v>0.40422442244224421</v>
+      </c>
+      <c r="C147">
+        <f>[1]Sheet1!C15</f>
+        <v>0.46937293729372931</v>
+      </c>
+      <c r="D147">
+        <f>[1]Sheet1!D15</f>
+        <v>0.45485148514851481</v>
+      </c>
+      <c r="E147">
+        <f>[1]Sheet1!E15</f>
+        <v>0.46478547854785479</v>
+      </c>
+      <c r="F147">
+        <f>[1]Sheet1!F15</f>
+        <v>0.43280528052805273</v>
+      </c>
+      <c r="G147">
+        <f>[1]Sheet1!G15</f>
+        <v>0.43623762376237629</v>
+      </c>
+      <c r="H147">
+        <f>[1]Sheet1!H15</f>
+        <v>0.45689768976897688</v>
+      </c>
+      <c r="I147">
+        <f>[1]Sheet1!I15</f>
+        <v>0.68306930693069312</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" t="str">
+        <f>[1]Sheet1!A16</f>
+        <v>map_cut_10</v>
+      </c>
+      <c r="B148">
+        <f>[1]Sheet1!B16</f>
+        <v>0.4155209806694955</v>
+      </c>
+      <c r="C148">
+        <f>[1]Sheet1!C16</f>
+        <v>0.47794593745088798</v>
+      </c>
+      <c r="D148">
+        <f>[1]Sheet1!D16</f>
+        <v>0.46118890460474621</v>
+      </c>
+      <c r="E148">
+        <f>[1]Sheet1!E16</f>
+        <v>0.47417256011315417</v>
+      </c>
+      <c r="F148">
+        <f>[1]Sheet1!F16</f>
+        <v>0.44110639635392113</v>
+      </c>
+      <c r="G148">
+        <f>[1]Sheet1!G16</f>
+        <v>0.44461260411755471</v>
+      </c>
+      <c r="H148">
+        <f>[1]Sheet1!H16</f>
+        <v>0.46161873330190162</v>
+      </c>
+      <c r="I148">
+        <f>[1]Sheet1!I16</f>
+        <v>0.68479019330504476</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" t="str">
+        <f>[1]Sheet1!A17</f>
+        <v>map_cut_100</v>
+      </c>
+      <c r="B149">
+        <f>[1]Sheet1!B17</f>
+        <v>0.42488362742894498</v>
+      </c>
+      <c r="C149">
+        <f>[1]Sheet1!C17</f>
+        <v>0.4872134221457734</v>
+      </c>
+      <c r="D149">
+        <f>[1]Sheet1!D17</f>
+        <v>0.469563637924027</v>
+      </c>
+      <c r="E149">
+        <f>[1]Sheet1!E17</f>
+        <v>0.4822241441449609</v>
+      </c>
+      <c r="F149">
+        <f>[1]Sheet1!F17</f>
+        <v>0.4498824784876414</v>
+      </c>
+      <c r="G149">
+        <f>[1]Sheet1!G17</f>
+        <v>0.45234578405123521</v>
+      </c>
+      <c r="H149">
+        <f>[1]Sheet1!H17</f>
+        <v>0.47104781340409702</v>
+      </c>
+      <c r="I149">
+        <f>[1]Sheet1!I17</f>
+        <v>0.68536277648194477</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" t="str">
+        <f>[1]Sheet1!A18</f>
+        <v>success_1</v>
+      </c>
+      <c r="B150">
+        <f>[1]Sheet1!B18</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C150">
+        <f>[1]Sheet1!C18</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D150">
+        <f>[1]Sheet1!D18</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E150">
+        <f>[1]Sheet1!E18</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F150">
+        <f>[1]Sheet1!F18</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G150">
+        <f>[1]Sheet1!G18</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H150">
+        <f>[1]Sheet1!H18</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I150">
+        <f>[1]Sheet1!I18</f>
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" t="str">
+        <f>[1]Sheet1!A19</f>
+        <v>success_5</v>
+      </c>
+      <c r="B151">
+        <f>[1]Sheet1!B19</f>
+        <v>0.52475247524752477</v>
+      </c>
+      <c r="C151">
+        <f>[1]Sheet1!C19</f>
+        <v>0.56831683168316827</v>
+      </c>
+      <c r="D151">
+        <f>[1]Sheet1!D19</f>
+        <v>0.55049504950495054</v>
+      </c>
+      <c r="E151">
+        <f>[1]Sheet1!E19</f>
+        <v>0.55841584158415847</v>
+      </c>
+      <c r="F151">
+        <f>[1]Sheet1!F19</f>
+        <v>0.53861386138613865</v>
+      </c>
+      <c r="G151">
+        <f>[1]Sheet1!G19</f>
+        <v>0.52871287128712874</v>
+      </c>
+      <c r="H151">
+        <f>[1]Sheet1!H19</f>
+        <v>0.56633663366336628</v>
+      </c>
+      <c r="I151">
+        <f>[1]Sheet1!I19</f>
+        <v>0.78613861386138617</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" t="str">
+        <f>[1]Sheet1!A20</f>
+        <v>success_10</v>
+      </c>
+      <c r="B152">
+        <f>[1]Sheet1!B20</f>
+        <v>0.60792079207920791</v>
+      </c>
+      <c r="C152">
+        <f>[1]Sheet1!C20</f>
+        <v>0.63168316831683169</v>
+      </c>
+      <c r="D152">
+        <f>[1]Sheet1!D20</f>
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="E152">
+        <f>[1]Sheet1!E20</f>
+        <v>0.62970297029702971</v>
+      </c>
+      <c r="F152">
+        <f>[1]Sheet1!F20</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="G152">
+        <f>[1]Sheet1!G20</f>
+        <v>0.58811881188118809</v>
+      </c>
+      <c r="H152">
+        <f>[1]Sheet1!H20</f>
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="I152">
+        <f>[1]Sheet1!I20</f>
+        <v>0.79801980198019806</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" t="str">
+        <f>[1]Sheet1!A21</f>
+        <v>success_100</v>
+      </c>
+      <c r="B153">
+        <f>[1]Sheet1!B21</f>
+        <v>0.80990099009900995</v>
+      </c>
+      <c r="C153">
+        <f>[1]Sheet1!C21</f>
+        <v>0.82178217821782185</v>
+      </c>
+      <c r="D153">
+        <f>[1]Sheet1!D21</f>
+        <v>0.80198019801980203</v>
+      </c>
+      <c r="E153">
+        <f>[1]Sheet1!E21</f>
+        <v>0.81782178217821788</v>
+      </c>
+      <c r="F153">
+        <f>[1]Sheet1!F21</f>
+        <v>0.80594059405940599</v>
+      </c>
+      <c r="G153">
+        <f>[1]Sheet1!G21</f>
+        <v>0.79603960396039608</v>
+      </c>
+      <c r="H153">
+        <f>[1]Sheet1!H21</f>
+        <v>0.8158415841584159</v>
+      </c>
+      <c r="I153">
+        <f>[1]Sheet1!I21</f>
+        <v>0.81782178217821788</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4570,10 +6561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8DF60C-3A99-4B9F-820E-01296226828F}">
-  <dimension ref="A1:W83"/>
+  <dimension ref="A1:W105"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView topLeftCell="Q65" workbookViewId="0">
+      <selection activeCell="W93" sqref="W93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8862,7 +10853,7 @@
         <v>2.1445498749811001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -8891,7 +10882,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -8920,7 +10911,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -8947,6 +10938,1083 @@
       </c>
       <c r="I83">
         <v>1.2463492063492E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K85" t="str">
+        <f>[2]Sheet1!A1</f>
+        <v>metric</v>
+      </c>
+      <c r="L85" t="str">
+        <f>[2]Sheet1!B1</f>
+        <v>P_1</v>
+      </c>
+      <c r="M85" t="str">
+        <f>[2]Sheet1!C1</f>
+        <v>P_5</v>
+      </c>
+      <c r="N85" t="str">
+        <f>[2]Sheet1!D1</f>
+        <v>P_10</v>
+      </c>
+      <c r="O85" t="str">
+        <f>[2]Sheet1!F1</f>
+        <v>recall_1</v>
+      </c>
+      <c r="P85" t="str">
+        <f>[2]Sheet1!G1</f>
+        <v>recall_5</v>
+      </c>
+      <c r="Q85" t="str">
+        <f>[2]Sheet1!H1</f>
+        <v>recall_10</v>
+      </c>
+      <c r="R85" t="str">
+        <f>[2]Sheet1!J1</f>
+        <v>ndcg_cut_1</v>
+      </c>
+      <c r="S85" t="str">
+        <f>[2]Sheet1!K1</f>
+        <v>ndcg_cut_5</v>
+      </c>
+      <c r="T85" t="str">
+        <f>[2]Sheet1!L1</f>
+        <v>ndcg_cut_10</v>
+      </c>
+      <c r="U85" t="str">
+        <f>[2]Sheet1!N1</f>
+        <v>map_cut_1</v>
+      </c>
+      <c r="V85" t="str">
+        <f>[2]Sheet1!O1</f>
+        <v>map_cut_5</v>
+      </c>
+      <c r="W85" t="str">
+        <f>[2]Sheet1!P1</f>
+        <v>map_cut_10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C86">
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D86">
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E86">
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F86">
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G86">
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H86">
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I86">
+        <v>0.598019801980198</v>
+      </c>
+      <c r="K86" t="str">
+        <f>[2]Sheet1!A2</f>
+        <v>cat</v>
+      </c>
+      <c r="L86">
+        <f>[2]Sheet1!B2</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="M86">
+        <f>[2]Sheet1!C2</f>
+        <v>0.10495049504950479</v>
+      </c>
+      <c r="N86">
+        <f>[2]Sheet1!D2</f>
+        <v>6.07920792079207E-2</v>
+      </c>
+      <c r="O86">
+        <f>[2]Sheet1!F2</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="P86">
+        <f>[2]Sheet1!G2</f>
+        <v>0.52475247524752477</v>
+      </c>
+      <c r="Q86">
+        <f>[2]Sheet1!H2</f>
+        <v>0.60792079207920791</v>
+      </c>
+      <c r="R86">
+        <f>[2]Sheet1!J2</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="S86">
+        <f>[2]Sheet1!K2</f>
+        <v>0.43433685881132428</v>
+      </c>
+      <c r="T86">
+        <f>[2]Sheet1!L2</f>
+        <v>0.46142184532764291</v>
+      </c>
+      <c r="U86">
+        <f>[2]Sheet1!N2</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="V86">
+        <f>[2]Sheet1!O2</f>
+        <v>0.40422442244224421</v>
+      </c>
+      <c r="W86">
+        <f>[2]Sheet1!P2</f>
+        <v>0.4155209806694955</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87">
+        <v>0.10495049504950479</v>
+      </c>
+      <c r="C87">
+        <v>0.1136633663366335</v>
+      </c>
+      <c r="D87">
+        <v>0.11009900990099</v>
+      </c>
+      <c r="E87">
+        <v>0.1116831683168316</v>
+      </c>
+      <c r="F87">
+        <v>0.1077227722772276</v>
+      </c>
+      <c r="G87">
+        <v>0.1057425742574256</v>
+      </c>
+      <c r="H87">
+        <v>0.1132673267326731</v>
+      </c>
+      <c r="I87">
+        <v>0.1572277227722769</v>
+      </c>
+      <c r="K87" t="str">
+        <f>[2]Sheet1!A3</f>
+        <v>arabic.cat</v>
+      </c>
+      <c r="L87">
+        <f>[2]Sheet1!B3</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="M87">
+        <f>[2]Sheet1!C3</f>
+        <v>0.1136633663366335</v>
+      </c>
+      <c r="N87">
+        <f>[2]Sheet1!D3</f>
+        <v>6.3168316831683002E-2</v>
+      </c>
+      <c r="O87">
+        <f>[2]Sheet1!F3</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="P87">
+        <f>[2]Sheet1!G3</f>
+        <v>0.56831683168316827</v>
+      </c>
+      <c r="Q87">
+        <f>[2]Sheet1!H3</f>
+        <v>0.63168316831683169</v>
+      </c>
+      <c r="R87">
+        <f>[2]Sheet1!J3</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="S87">
+        <f>[2]Sheet1!K3</f>
+        <v>0.49393158719216779</v>
+      </c>
+      <c r="T87">
+        <f>[2]Sheet1!L3</f>
+        <v>0.51453621143316575</v>
+      </c>
+      <c r="U87">
+        <f>[2]Sheet1!N3</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="V87">
+        <f>[2]Sheet1!O3</f>
+        <v>0.46937293729372931</v>
+      </c>
+      <c r="W87">
+        <f>[2]Sheet1!P3</f>
+        <v>0.47794593745088798</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>6.07920792079207E-2</v>
+      </c>
+      <c r="C88">
+        <v>6.3168316831683002E-2</v>
+      </c>
+      <c r="D88">
+        <v>6.0198019801980099E-2</v>
+      </c>
+      <c r="E88">
+        <v>6.2970297029702901E-2</v>
+      </c>
+      <c r="F88">
+        <v>5.9801980198019702E-2</v>
+      </c>
+      <c r="G88">
+        <v>5.8811881188118698E-2</v>
+      </c>
+      <c r="H88">
+        <v>6.0198019801980099E-2</v>
+      </c>
+      <c r="I88">
+        <v>7.9801980198019595E-2</v>
+      </c>
+      <c r="K88" t="str">
+        <f>[2]Sheet1!A4</f>
+        <v>german.cat</v>
+      </c>
+      <c r="L88">
+        <f>[2]Sheet1!B4</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="M88">
+        <f>[2]Sheet1!C4</f>
+        <v>0.11009900990099</v>
+      </c>
+      <c r="N88">
+        <f>[2]Sheet1!D4</f>
+        <v>6.0198019801980099E-2</v>
+      </c>
+      <c r="O88">
+        <f>[2]Sheet1!F4</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="P88">
+        <f>[2]Sheet1!G4</f>
+        <v>0.55049504950495054</v>
+      </c>
+      <c r="Q88">
+        <f>[2]Sheet1!H4</f>
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="R88">
+        <f>[2]Sheet1!J4</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="S88">
+        <f>[2]Sheet1!K4</f>
+        <v>0.47867078650248568</v>
+      </c>
+      <c r="T88">
+        <f>[2]Sheet1!L4</f>
+        <v>0.49479441345825409</v>
+      </c>
+      <c r="U88">
+        <f>[2]Sheet1!N4</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="V88">
+        <f>[2]Sheet1!O4</f>
+        <v>0.45485148514851481</v>
+      </c>
+      <c r="W88">
+        <f>[2]Sheet1!P4</f>
+        <v>0.46118890460474621</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89">
+        <v>8.0990099009900993E-3</v>
+      </c>
+      <c r="C89">
+        <v>8.2178217821782008E-3</v>
+      </c>
+      <c r="D89">
+        <v>8.0198019801979992E-3</v>
+      </c>
+      <c r="E89">
+        <v>8.1782178217821005E-3</v>
+      </c>
+      <c r="F89">
+        <v>8.0594059405940006E-3</v>
+      </c>
+      <c r="G89">
+        <v>7.9603960396038998E-3</v>
+      </c>
+      <c r="H89">
+        <v>8.1584158415840997E-3</v>
+      </c>
+      <c r="I89">
+        <v>8.1782178217821005E-3</v>
+      </c>
+      <c r="K89" t="str">
+        <f>[2]Sheet1!A5</f>
+        <v>french.cat</v>
+      </c>
+      <c r="L89">
+        <f>[2]Sheet1!B5</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="M89">
+        <f>[2]Sheet1!C5</f>
+        <v>0.1116831683168316</v>
+      </c>
+      <c r="N89">
+        <f>[2]Sheet1!D5</f>
+        <v>6.2970297029702901E-2</v>
+      </c>
+      <c r="O89">
+        <f>[2]Sheet1!F5</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="P89">
+        <f>[2]Sheet1!G5</f>
+        <v>0.55841584158415847</v>
+      </c>
+      <c r="Q89">
+        <f>[2]Sheet1!H5</f>
+        <v>0.62970297029702971</v>
+      </c>
+      <c r="R89">
+        <f>[2]Sheet1!J5</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="S89">
+        <f>[2]Sheet1!K5</f>
+        <v>0.48832212190279489</v>
+      </c>
+      <c r="T89">
+        <f>[2]Sheet1!L5</f>
+        <v>0.51124006193511495</v>
+      </c>
+      <c r="U89">
+        <f>[2]Sheet1!N5</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="V89">
+        <f>[2]Sheet1!O5</f>
+        <v>0.46478547854785479</v>
+      </c>
+      <c r="W89">
+        <f>[2]Sheet1!P5</f>
+        <v>0.47417256011315417</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C90">
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D90">
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E90">
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F90">
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G90">
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H90">
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I90">
+        <v>0.598019801980198</v>
+      </c>
+      <c r="K90" t="str">
+        <f>[2]Sheet1!A6</f>
+        <v>farsi.cat</v>
+      </c>
+      <c r="L90">
+        <f>[2]Sheet1!B6</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="M90">
+        <f>[2]Sheet1!C6</f>
+        <v>0.1077227722772276</v>
+      </c>
+      <c r="N90">
+        <f>[2]Sheet1!D6</f>
+        <v>5.9801980198019702E-2</v>
+      </c>
+      <c r="O90">
+        <f>[2]Sheet1!F6</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="P90">
+        <f>[2]Sheet1!G6</f>
+        <v>0.53861386138613865</v>
+      </c>
+      <c r="Q90">
+        <f>[2]Sheet1!H6</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="R90">
+        <f>[2]Sheet1!J6</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="S90">
+        <f>[2]Sheet1!K6</f>
+        <v>0.45923120656909389</v>
+      </c>
+      <c r="T90">
+        <f>[2]Sheet1!L6</f>
+        <v>0.47881210170055832</v>
+      </c>
+      <c r="U90">
+        <f>[2]Sheet1!N6</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="V90">
+        <f>[2]Sheet1!O6</f>
+        <v>0.43280528052805273</v>
+      </c>
+      <c r="W90">
+        <f>[2]Sheet1!P6</f>
+        <v>0.44110639635392113</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91">
+        <v>0.52475247524752477</v>
+      </c>
+      <c r="C91">
+        <v>0.56831683168316827</v>
+      </c>
+      <c r="D91">
+        <v>0.55049504950495054</v>
+      </c>
+      <c r="E91">
+        <v>0.55841584158415847</v>
+      </c>
+      <c r="F91">
+        <v>0.53861386138613865</v>
+      </c>
+      <c r="G91">
+        <v>0.52871287128712874</v>
+      </c>
+      <c r="H91">
+        <v>0.56633663366336628</v>
+      </c>
+      <c r="I91">
+        <v>0.78613861386138617</v>
+      </c>
+      <c r="K91" t="str">
+        <f>[2]Sheet1!A7</f>
+        <v>chinese.cat</v>
+      </c>
+      <c r="L91">
+        <f>[2]Sheet1!B7</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="M91">
+        <f>[2]Sheet1!C7</f>
+        <v>0.1057425742574256</v>
+      </c>
+      <c r="N91">
+        <f>[2]Sheet1!D7</f>
+        <v>5.8811881188118698E-2</v>
+      </c>
+      <c r="O91">
+        <f>[2]Sheet1!F7</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="P91">
+        <f>[2]Sheet1!G7</f>
+        <v>0.52871287128712874</v>
+      </c>
+      <c r="Q91">
+        <f>[2]Sheet1!H7</f>
+        <v>0.58811881188118809</v>
+      </c>
+      <c r="R91">
+        <f>[2]Sheet1!J7</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="S91">
+        <f>[2]Sheet1!K7</f>
+        <v>0.45956591316347828</v>
+      </c>
+      <c r="T91">
+        <f>[2]Sheet1!L7</f>
+        <v>0.479215482410146</v>
+      </c>
+      <c r="U91">
+        <f>[2]Sheet1!N7</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="V91">
+        <f>[2]Sheet1!O7</f>
+        <v>0.43623762376237629</v>
+      </c>
+      <c r="W91">
+        <f>[2]Sheet1!P7</f>
+        <v>0.44461260411755471</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92">
+        <v>0.60792079207920791</v>
+      </c>
+      <c r="C92">
+        <v>0.63168316831683169</v>
+      </c>
+      <c r="D92">
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="E92">
+        <v>0.62970297029702971</v>
+      </c>
+      <c r="F92">
+        <v>0.598019801980198</v>
+      </c>
+      <c r="G92">
+        <v>0.58811881188118809</v>
+      </c>
+      <c r="H92">
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="I92">
+        <v>0.79801980198019806</v>
+      </c>
+      <c r="K92" t="str">
+        <f>[2]Sheet1!A8</f>
+        <v>spanish.cat</v>
+      </c>
+      <c r="L92">
+        <f>[2]Sheet1!B8</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="M92">
+        <f>[2]Sheet1!C8</f>
+        <v>0.1132673267326731</v>
+      </c>
+      <c r="N92">
+        <f>[2]Sheet1!D8</f>
+        <v>6.0198019801980099E-2</v>
+      </c>
+      <c r="O92">
+        <f>[2]Sheet1!F8</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="P92">
+        <f>[2]Sheet1!G8</f>
+        <v>0.56633663366336628</v>
+      </c>
+      <c r="Q92">
+        <f>[2]Sheet1!H8</f>
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="R92">
+        <f>[2]Sheet1!J8</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="S92">
+        <f>[2]Sheet1!K8</f>
+        <v>0.4841750282211964</v>
+      </c>
+      <c r="T92">
+        <f>[2]Sheet1!L8</f>
+        <v>0.49566258216036968</v>
+      </c>
+      <c r="U92">
+        <f>[2]Sheet1!N8</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="V92">
+        <f>[2]Sheet1!O8</f>
+        <v>0.45689768976897688</v>
+      </c>
+      <c r="W92">
+        <f>[2]Sheet1!P8</f>
+        <v>0.46161873330190162</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93">
+        <v>0.80990099009900995</v>
+      </c>
+      <c r="C93">
+        <v>0.82178217821782185</v>
+      </c>
+      <c r="D93">
+        <v>0.80198019801980203</v>
+      </c>
+      <c r="E93">
+        <v>0.81782178217821788</v>
+      </c>
+      <c r="F93">
+        <v>0.80594059405940599</v>
+      </c>
+      <c r="G93">
+        <v>0.79603960396039608</v>
+      </c>
+      <c r="H93">
+        <v>0.8158415841584159</v>
+      </c>
+      <c r="I93">
+        <v>0.81782178217821788</v>
+      </c>
+      <c r="K93" t="str">
+        <f>[2]Sheet1!A9</f>
+        <v>all.cat</v>
+      </c>
+      <c r="L93">
+        <f>[2]Sheet1!B9</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="M93">
+        <f>[2]Sheet1!C9</f>
+        <v>0.1572277227722769</v>
+      </c>
+      <c r="N93">
+        <f>[2]Sheet1!D9</f>
+        <v>7.9801980198019595E-2</v>
+      </c>
+      <c r="O93">
+        <f>[2]Sheet1!F9</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="P93">
+        <f>[2]Sheet1!G9</f>
+        <v>0.78613861386138617</v>
+      </c>
+      <c r="Q93">
+        <f>[2]Sheet1!H9</f>
+        <v>0.79801980198019806</v>
+      </c>
+      <c r="R93">
+        <f>[2]Sheet1!J9</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="S93">
+        <f>[2]Sheet1!K9</f>
+        <v>0.70960729180542281</v>
+      </c>
+      <c r="T93">
+        <f>[2]Sheet1!L9</f>
+        <v>0.71358751120038144</v>
+      </c>
+      <c r="U93">
+        <f>[2]Sheet1!N9</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="V93">
+        <f>[2]Sheet1!O9</f>
+        <v>0.68306930693069312</v>
+      </c>
+      <c r="W93">
+        <f>[2]Sheet1!P9</f>
+        <v>0.68479019330504476</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94">
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C94">
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D94">
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E94">
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F94">
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G94">
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H94">
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I94">
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95">
+        <v>0.43433685881132428</v>
+      </c>
+      <c r="C95">
+        <v>0.49393158719216779</v>
+      </c>
+      <c r="D95">
+        <v>0.47867078650248568</v>
+      </c>
+      <c r="E95">
+        <v>0.48832212190279489</v>
+      </c>
+      <c r="F95">
+        <v>0.45923120656909389</v>
+      </c>
+      <c r="G95">
+        <v>0.45956591316347828</v>
+      </c>
+      <c r="H95">
+        <v>0.4841750282211964</v>
+      </c>
+      <c r="I95">
+        <v>0.70960729180542281</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96">
+        <v>0.46142184532764291</v>
+      </c>
+      <c r="C96">
+        <v>0.51453621143316575</v>
+      </c>
+      <c r="D96">
+        <v>0.49479441345825409</v>
+      </c>
+      <c r="E96">
+        <v>0.51124006193511495</v>
+      </c>
+      <c r="F96">
+        <v>0.47881210170055832</v>
+      </c>
+      <c r="G96">
+        <v>0.479215482410146</v>
+      </c>
+      <c r="H96">
+        <v>0.49566258216036968</v>
+      </c>
+      <c r="I96">
+        <v>0.71358751120038144</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97">
+        <v>0.50529935513018653</v>
+      </c>
+      <c r="C97">
+        <v>0.55670661377860775</v>
+      </c>
+      <c r="D97">
+        <v>0.53687811583328249</v>
+      </c>
+      <c r="E97">
+        <v>0.55128375161457255</v>
+      </c>
+      <c r="F97">
+        <v>0.52282318292622265</v>
+      </c>
+      <c r="G97">
+        <v>0.52150583498395298</v>
+      </c>
+      <c r="H97">
+        <v>0.54132733999753324</v>
+      </c>
+      <c r="I97">
+        <v>0.71728765166300479</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>13</v>
+      </c>
+      <c r="B98">
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C98">
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D98">
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E98">
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F98">
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G98">
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H98">
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I98">
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99">
+        <v>0.40422442244224421</v>
+      </c>
+      <c r="C99">
+        <v>0.46937293729372931</v>
+      </c>
+      <c r="D99">
+        <v>0.45485148514851481</v>
+      </c>
+      <c r="E99">
+        <v>0.46478547854785479</v>
+      </c>
+      <c r="F99">
+        <v>0.43280528052805273</v>
+      </c>
+      <c r="G99">
+        <v>0.43623762376237629</v>
+      </c>
+      <c r="H99">
+        <v>0.45689768976897688</v>
+      </c>
+      <c r="I99">
+        <v>0.68306930693069312</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>15</v>
+      </c>
+      <c r="B100">
+        <v>0.4155209806694955</v>
+      </c>
+      <c r="C100">
+        <v>0.47794593745088798</v>
+      </c>
+      <c r="D100">
+        <v>0.46118890460474621</v>
+      </c>
+      <c r="E100">
+        <v>0.47417256011315417</v>
+      </c>
+      <c r="F100">
+        <v>0.44110639635392113</v>
+      </c>
+      <c r="G100">
+        <v>0.44461260411755471</v>
+      </c>
+      <c r="H100">
+        <v>0.46161873330190162</v>
+      </c>
+      <c r="I100">
+        <v>0.68479019330504476</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101">
+        <v>0.42488362742894498</v>
+      </c>
+      <c r="C101">
+        <v>0.4872134221457734</v>
+      </c>
+      <c r="D101">
+        <v>0.469563637924027</v>
+      </c>
+      <c r="E101">
+        <v>0.4822241441449609</v>
+      </c>
+      <c r="F101">
+        <v>0.4498824784876414</v>
+      </c>
+      <c r="G101">
+        <v>0.45234578405123521</v>
+      </c>
+      <c r="H101">
+        <v>0.47104781340409702</v>
+      </c>
+      <c r="I101">
+        <v>0.68536277648194477</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B102">
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="C102">
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="D102">
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="E102">
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="F102">
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="G102">
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="H102">
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="I102">
+        <v>0.598019801980198</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103">
+        <v>0.52475247524752477</v>
+      </c>
+      <c r="C103">
+        <v>0.56831683168316827</v>
+      </c>
+      <c r="D103">
+        <v>0.55049504950495054</v>
+      </c>
+      <c r="E103">
+        <v>0.55841584158415847</v>
+      </c>
+      <c r="F103">
+        <v>0.53861386138613865</v>
+      </c>
+      <c r="G103">
+        <v>0.52871287128712874</v>
+      </c>
+      <c r="H103">
+        <v>0.56633663366336628</v>
+      </c>
+      <c r="I103">
+        <v>0.78613861386138617</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104">
+        <v>0.60792079207920791</v>
+      </c>
+      <c r="C104">
+        <v>0.63168316831683169</v>
+      </c>
+      <c r="D104">
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="E104">
+        <v>0.62970297029702971</v>
+      </c>
+      <c r="F104">
+        <v>0.598019801980198</v>
+      </c>
+      <c r="G104">
+        <v>0.58811881188118809</v>
+      </c>
+      <c r="H104">
+        <v>0.60198019801980196</v>
+      </c>
+      <c r="I104">
+        <v>0.79801980198019806</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105">
+        <v>0.80990099009900995</v>
+      </c>
+      <c r="C105">
+        <v>0.82178217821782185</v>
+      </c>
+      <c r="D105">
+        <v>0.80198019801980203</v>
+      </c>
+      <c r="E105">
+        <v>0.81782178217821788</v>
+      </c>
+      <c r="F105">
+        <v>0.80594059405940599</v>
+      </c>
+      <c r="G105">
+        <v>0.79603960396039608</v>
+      </c>
+      <c r="H105">
+        <v>0.8158415841584159</v>
+      </c>
+      <c r="I105">
+        <v>0.81782178217821788</v>
       </c>
     </row>
   </sheetData>
@@ -8956,10 +12024,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3A18D2-30FF-4570-A5C2-4E4FB86528D4}">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8969,49 +12037,55 @@
     <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10" t="s">
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
       <c r="B2" s="4" t="s">
         <v>83</v>
       </c>
@@ -9084,8 +12158,20 @@
       <c r="Y2" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -9161,8 +12247,24 @@
       <c r="Y3" s="3">
         <v>1.2133333333329999E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3" s="2">
+        <f>[3]Sheet1!B2</f>
+        <v>0.33267326732673269</v>
+      </c>
+      <c r="AA3" s="2">
+        <f>[3]Sheet1!C2</f>
+        <v>0.52475247524752477</v>
+      </c>
+      <c r="AB3" s="2">
+        <f>[3]Sheet1!D2</f>
+        <v>0.43433685881132428</v>
+      </c>
+      <c r="AC3" s="2">
+        <f>[3]Sheet1!E2</f>
+        <v>0.40422442244224421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
@@ -9238,8 +12340,24 @@
       <c r="Y4" s="8">
         <v>1.5333333333333E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4" s="2">
+        <f>[3]Sheet1!B3</f>
+        <v>0.37227722772277227</v>
+      </c>
+      <c r="AA4" s="2">
+        <f>[3]Sheet1!C3</f>
+        <v>0.52871287128712874</v>
+      </c>
+      <c r="AB4" s="2">
+        <f>[3]Sheet1!D3</f>
+        <v>0.45956591316347828</v>
+      </c>
+      <c r="AC4" s="2">
+        <f>[3]Sheet1!E3</f>
+        <v>0.43623762376237629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -9315,8 +12433,24 @@
       <c r="Y5" s="3">
         <v>5.7142857142857101E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" s="2">
+        <f>[3]Sheet1!B4</f>
+        <v>0.37029702970297029</v>
+      </c>
+      <c r="AA5" s="2">
+        <f>[3]Sheet1!C4</f>
+        <v>0.53861386138613865</v>
+      </c>
+      <c r="AB5" s="2">
+        <f>[3]Sheet1!D4</f>
+        <v>0.45923120656909389</v>
+      </c>
+      <c r="AC5" s="2">
+        <f>[3]Sheet1!E4</f>
+        <v>0.43280528052805273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
@@ -9392,8 +12526,24 @@
       <c r="Y6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6" s="2">
+        <f>[3]Sheet1!B5</f>
+        <v>0.4138613861386139</v>
+      </c>
+      <c r="AA6" s="2">
+        <f>[3]Sheet1!C5</f>
+        <v>0.56831683168316827</v>
+      </c>
+      <c r="AB6" s="2">
+        <f>[3]Sheet1!D5</f>
+        <v>0.49393158719216779</v>
+      </c>
+      <c r="AC6" s="2">
+        <f>[3]Sheet1!E5</f>
+        <v>0.46937293729372931</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
@@ -9469,8 +12619,24 @@
       <c r="Y7" s="3">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z7" s="2">
+        <f>[3]Sheet1!B6</f>
+        <v>0.40396039603960399</v>
+      </c>
+      <c r="AA7" s="2">
+        <f>[3]Sheet1!C6</f>
+        <v>0.55841584158415847</v>
+      </c>
+      <c r="AB7" s="2">
+        <f>[3]Sheet1!D6</f>
+        <v>0.48832212190279489</v>
+      </c>
+      <c r="AC7" s="2">
+        <f>[3]Sheet1!E6</f>
+        <v>0.46478547854785479</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>71</v>
       </c>
@@ -9546,8 +12712,24 @@
       <c r="Y8" s="7">
         <v>2.2666666666666E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="2">
+        <f>[3]Sheet1!B7</f>
+        <v>0.39801980198019798</v>
+      </c>
+      <c r="AA8" s="2">
+        <f>[3]Sheet1!C7</f>
+        <v>0.55049504950495054</v>
+      </c>
+      <c r="AB8" s="2">
+        <f>[3]Sheet1!D7</f>
+        <v>0.47867078650248568</v>
+      </c>
+      <c r="AC8" s="2">
+        <f>[3]Sheet1!E7</f>
+        <v>0.45485148514851481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -9623,8 +12805,24 @@
       <c r="Y9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="2">
+        <f>[3]Sheet1!B8</f>
+        <v>0.39207920792079209</v>
+      </c>
+      <c r="AA9" s="2">
+        <f>[3]Sheet1!C8</f>
+        <v>0.56633663366336628</v>
+      </c>
+      <c r="AB9" s="2">
+        <f>[3]Sheet1!D8</f>
+        <v>0.4841750282211964</v>
+      </c>
+      <c r="AC9" s="2">
+        <f>[3]Sheet1!E8</f>
+        <v>0.45689768976897688</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -9700,8 +12898,24 @@
       <c r="Y10" s="3">
         <v>8.0000000000000004E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="2">
+        <f>[3]Sheet1!B9</f>
+        <v>0.598019801980198</v>
+      </c>
+      <c r="AA10" s="2">
+        <f>[3]Sheet1!C9</f>
+        <v>0.78613861386138617</v>
+      </c>
+      <c r="AB10" s="2">
+        <f>[3]Sheet1!D9</f>
+        <v>0.70960729180542281</v>
+      </c>
+      <c r="AC10" s="2">
+        <f>[3]Sheet1!E9</f>
+        <v>0.68306930693069312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -9728,7 +12942,8 @@
       <c r="Y11" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
cat is added to charts
</commit_message>
<xml_diff>
--- a/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
+++ b/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farinam\PycharmProjects\LADy\output\2015SB12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hfani/Github/fani-lab/LADy/main/output/2015SB12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604B6812-30DD-4FBB-8AD7-605BE20B00D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14C0CA5-B599-1B43-B728-DFCE5F18D4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,6 +368,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -436,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -458,20 +459,51 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2093,16 +2125,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DE02BE-45B7-4D8D-BCA0-35520325FAF3}">
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+    <sheetView topLeftCell="A117" workbookViewId="0">
       <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2131,7 +2163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2160,7 +2192,7 @@
         <v>0.21279999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2189,7 +2221,7 @@
         <v>8.89599999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2218,7 +2250,7 @@
         <v>5.2959999999999903E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2247,7 +2279,7 @@
         <v>1.0208E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2276,7 +2308,7 @@
         <v>0.152106666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2305,7 +2337,7 @@
         <v>0.29861333333333301</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2334,7 +2366,7 @@
         <v>0.35119999999999901</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2363,7 +2395,7 @@
         <v>0.59628571428571397</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2392,7 +2424,7 @@
         <v>0.21279999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2421,7 +2453,7 @@
         <v>0.25147113938973098</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2450,7 +2482,7 @@
         <v>0.27023987258530402</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2479,7 +2511,7 @@
         <v>0.33064506362917101</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2508,7 +2540,7 @@
         <v>0.152106666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2537,7 +2569,7 @@
         <v>0.21400177777777701</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2566,7 +2598,7 @@
         <v>0.22167585185185101</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2595,7 +2627,7 @@
         <v>0.23398065524836001</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2624,7 +2656,7 @@
         <v>0.21279999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2653,7 +2685,7 @@
         <v>0.38879999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2682,7 +2714,7 @@
         <v>0.46079999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2711,7 +2743,7 @@
         <v>0.74879999999999902</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2772,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2769,7 +2801,7 @@
         <v>0.21920000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -2798,7 +2830,7 @@
         <v>7.9039999999999902E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2827,7 +2859,7 @@
         <v>4.65599999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2856,7 +2888,7 @@
         <v>1.0288E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -2885,7 +2917,7 @@
         <v>0.15122666666666601</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -2914,7 +2946,7 @@
         <v>0.247013333333333</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2943,7 +2975,7 @@
         <v>0.28414857142857097</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2972,7 +3004,7 @@
         <v>0.59225714285714204</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -3001,7 +3033,7 @@
         <v>0.21920000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -3030,7 +3062,7 @@
         <v>0.22629866399950399</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -3059,7 +3091,7 @@
         <v>0.239501257872131</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3088,7 +3120,7 @@
         <v>0.31122066321356701</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -3117,7 +3149,7 @@
         <v>0.15122666666666601</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3146,7 +3178,7 @@
         <v>0.194193333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -3175,7 +3207,7 @@
         <v>0.19952719274376399</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -3204,7 +3236,7 @@
         <v>0.21316044074708701</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -3233,7 +3265,7 @@
         <v>0.21920000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -3262,7 +3294,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -3291,7 +3323,7 @@
         <v>0.40960000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -3320,7 +3352,7 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -3349,7 +3381,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -3378,7 +3410,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -3407,7 +3439,7 @@
         <v>0.11359999999999899</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -3436,7 +3468,7 @@
         <v>6.7359999999999906E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3465,7 +3497,7 @@
         <v>9.8720000000000006E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -3494,7 +3526,7 @@
         <v>0.17106666666666601</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -3523,7 +3555,7 @@
         <v>0.374373333333333</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -3552,7 +3584,7 @@
         <v>0.43401523809523801</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -3581,7 +3613,7 @@
         <v>0.58357333333333306</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -3610,7 +3642,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3639,7 +3671,7 @@
         <v>0.31040362405493099</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -3668,7 +3700,7 @@
         <v>0.33182754446553497</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -3697,7 +3729,7 @@
         <v>0.37248576969911001</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -3726,7 +3758,7 @@
         <v>0.17106666666666601</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3755,7 +3787,7 @@
         <v>0.25776888888888799</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3784,7 +3816,7 @@
         <v>0.26755987301587197</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -3813,7 +3845,7 @@
         <v>0.277474289415583</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -3842,7 +3874,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -3871,7 +3903,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -3900,7 +3932,7 @@
         <v>0.56640000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -3929,7 +3961,7 @@
         <v>0.74079999999999901</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -3958,7 +3990,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -3987,7 +4019,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -4016,7 +4048,7 @@
         <v>2.656E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -4045,7 +4077,7 @@
         <v>1.7440000000000001E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -4074,7 +4106,7 @@
         <v>6.0480000000000004E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -4103,7 +4135,7 @@
         <v>2.1919999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -4132,7 +4164,7 @@
         <v>7.5653333333333295E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -4161,7 +4193,7 @@
         <v>9.7641904761904694E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -4190,7 +4222,7 @@
         <v>0.35544761904761901</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -4219,7 +4251,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -4248,7 +4280,7 @@
         <v>5.8043532868121799E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -4277,7 +4309,7 @@
         <v>6.6125296616557E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -4306,7 +4338,7 @@
         <v>0.121637011287014</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -4335,7 +4367,7 @@
         <v>2.1919999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4364,7 +4396,7 @@
         <v>4.1966666666666597E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -4393,7 +4425,7 @@
         <v>4.5236039304610703E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -4422,7 +4454,7 @@
         <v>5.3798705533092003E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -4451,7 +4483,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -4480,7 +4512,7 @@
         <v>0.12640000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -4509,7 +4541,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>20</v>
       </c>
@@ -4538,7 +4570,7 @@
         <v>0.50560000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -4567,7 +4599,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -4596,7 +4628,7 @@
         <v>2.24E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -4625,7 +4657,7 @@
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -4654,7 +4686,7 @@
         <v>2.5919999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>4</v>
       </c>
@@ -4683,7 +4715,7 @@
         <v>7.9360000000000003E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -4712,7 +4744,7 @@
         <v>1.38438095238095E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -4741,7 +4773,7 @@
         <v>7.3100952380952294E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -4770,7 +4802,7 @@
         <v>0.14519619047619001</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -4799,7 +4831,7 @@
         <v>0.45667238095238</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -4828,7 +4860,7 @@
         <v>2.24E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4857,7 +4889,7 @@
         <v>4.78374663687973E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -4886,7 +4918,7 @@
         <v>7.3699174623340302E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -4915,7 +4947,7 @@
         <v>0.14382513812276401</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -4944,7 +4976,7 @@
         <v>1.38438095238095E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -4973,7 +5005,7 @@
         <v>3.1792063492063399E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -5002,7 +5034,7 @@
         <v>4.1415449735449701E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -5031,7 +5063,7 @@
         <v>5.3546239917164999E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>17</v>
       </c>
@@ -5060,7 +5092,7 @@
         <v>2.24E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -5089,7 +5121,7 @@
         <v>0.1216</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>19</v>
       </c>
@@ -5118,7 +5150,7 @@
         <v>0.23680000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>20</v>
       </c>
@@ -5147,7 +5179,7 @@
         <v>0.62080000000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -5176,7 +5208,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -5205,7 +5237,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -5234,7 +5266,7 @@
         <v>3.2000000000000003E-4</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>3</v>
       </c>
@@ -5263,7 +5295,7 @@
         <v>6.4000000000000005E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>4</v>
       </c>
@@ -5292,7 +5324,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -5321,7 +5353,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -5350,7 +5382,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -5379,7 +5411,7 @@
         <v>4.1066666666665997E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -5408,7 +5440,7 @@
         <v>4.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -5437,7 +5469,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -5466,7 +5498,7 @@
         <v>9.8103550842470002E-4</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -5495,7 +5527,7 @@
         <v>2.1445498749811001E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>12</v>
       </c>
@@ -5524,7 +5556,7 @@
         <v>2.3114484496906998E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -5553,7 +5585,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>14</v>
       </c>
@@ -5582,7 +5614,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -5611,7 +5643,7 @@
         <v>1.2463492063492E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>16</v>
       </c>
@@ -5640,7 +5672,7 @@
         <v>1.2744973544973001E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -5669,7 +5701,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>18</v>
       </c>
@@ -5698,7 +5730,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>19</v>
       </c>
@@ -5727,7 +5759,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>20</v>
       </c>
@@ -5756,7 +5788,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="str">
         <f>[1]Sheet1!A1</f>
         <v>metric</v>
@@ -5794,7 +5826,7 @@
         <v>pes_Arab.zho_Hans.deu_Latn.arb_Arab.fra_Latn.spa_Latn.cat.0.0</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="str">
         <f>[1]Sheet1!A2</f>
         <v>P_1</v>
@@ -5832,7 +5864,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="str">
         <f>[1]Sheet1!A3</f>
         <v>P_5</v>
@@ -5870,7 +5902,7 @@
         <v>0.1572277227722769</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="str">
         <f>[1]Sheet1!A4</f>
         <v>P_10</v>
@@ -5908,7 +5940,7 @@
         <v>7.9801980198019595E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="str">
         <f>[1]Sheet1!A5</f>
         <v>P_100</v>
@@ -5946,7 +5978,7 @@
         <v>8.1782178217821005E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="str">
         <f>[1]Sheet1!A6</f>
         <v>recall_1</v>
@@ -5984,7 +6016,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="str">
         <f>[1]Sheet1!A7</f>
         <v>recall_5</v>
@@ -6022,7 +6054,7 @@
         <v>0.78613861386138617</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="str">
         <f>[1]Sheet1!A8</f>
         <v>recall_10</v>
@@ -6060,7 +6092,7 @@
         <v>0.79801980198019806</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="str">
         <f>[1]Sheet1!A9</f>
         <v>recall_100</v>
@@ -6098,7 +6130,7 @@
         <v>0.81782178217821788</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="str">
         <f>[1]Sheet1!A10</f>
         <v>ndcg_cut_1</v>
@@ -6136,7 +6168,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="str">
         <f>[1]Sheet1!A11</f>
         <v>ndcg_cut_5</v>
@@ -6174,7 +6206,7 @@
         <v>0.70960729180542281</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="str">
         <f>[1]Sheet1!A12</f>
         <v>ndcg_cut_10</v>
@@ -6212,7 +6244,7 @@
         <v>0.71358751120038144</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="str">
         <f>[1]Sheet1!A13</f>
         <v>ndcg_cut_100</v>
@@ -6250,7 +6282,7 @@
         <v>0.71728765166300479</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="str">
         <f>[1]Sheet1!A14</f>
         <v>map_cut_1</v>
@@ -6288,7 +6320,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="str">
         <f>[1]Sheet1!A15</f>
         <v>map_cut_5</v>
@@ -6326,7 +6358,7 @@
         <v>0.68306930693069312</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="str">
         <f>[1]Sheet1!A16</f>
         <v>map_cut_10</v>
@@ -6364,7 +6396,7 @@
         <v>0.68479019330504476</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="str">
         <f>[1]Sheet1!A17</f>
         <v>map_cut_100</v>
@@ -6402,7 +6434,7 @@
         <v>0.68536277648194477</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="str">
         <f>[1]Sheet1!A18</f>
         <v>success_1</v>
@@ -6440,7 +6472,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="str">
         <f>[1]Sheet1!A19</f>
         <v>success_5</v>
@@ -6478,7 +6510,7 @@
         <v>0.78613861386138617</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="str">
         <f>[1]Sheet1!A20</f>
         <v>success_10</v>
@@ -6516,7 +6548,7 @@
         <v>0.79801980198019806</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="str">
         <f>[1]Sheet1!A21</f>
         <v>success_100</v>
@@ -6563,16 +6595,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8DF60C-3A99-4B9F-820E-01296226828F}">
   <dimension ref="A1:W105"/>
   <sheetViews>
-    <sheetView topLeftCell="Q65" workbookViewId="0">
-      <selection activeCell="W93" sqref="W93"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6640,7 +6672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6708,7 +6740,7 @@
         <v>0.21275286772486701</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6776,7 +6808,7 @@
         <v>0.192248296296296</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6844,7 +6876,7 @@
         <v>0.200167809523809</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -6912,7 +6944,7 @@
         <v>0.22157174603174501</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -6980,7 +7012,7 @@
         <v>0.198939978835978</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -7048,7 +7080,7 @@
         <v>0.20257053665910801</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -7116,7 +7148,7 @@
         <v>0.21551279365079301</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -7184,7 +7216,7 @@
         <v>0.22167585185185101</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -7213,7 +7245,7 @@
         <v>0.27023987258530402</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -7242,7 +7274,7 @@
         <v>0.152106666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -7271,7 +7303,7 @@
         <v>0.21400177777777701</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -7300,7 +7332,7 @@
         <v>0.22167585185185101</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -7368,7 +7400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -7436,7 +7468,7 @@
         <v>4.4582222222222197E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -7504,7 +7536,7 @@
         <v>4.8447830687830602E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -7572,7 +7604,7 @@
         <v>5.1454285714285702E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -7640,7 +7672,7 @@
         <v>6.1332275132275099E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -7708,7 +7740,7 @@
         <v>6.2814126984126903E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -7776,7 +7808,7 @@
         <v>5.6631746031745998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -7844,7 +7876,7 @@
         <v>3.8382751322751298E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -7912,7 +7944,7 @@
         <v>0.19952719274376399</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -7941,7 +7973,7 @@
         <v>0.239501257872131</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -7970,7 +8002,7 @@
         <v>0.15122666666666601</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -7999,7 +8031,7 @@
         <v>0.194193333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -8028,7 +8060,7 @@
         <v>0.19952719274376399</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -8096,7 +8128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -8164,7 +8196,7 @@
         <v>0.25492650793650701</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -8232,7 +8264,7 @@
         <v>0.24628016931216901</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -8300,7 +8332,7 @@
         <v>0.26086635978835898</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -8368,7 +8400,7 @@
         <v>0.26959068783068701</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -8436,7 +8468,7 @@
         <v>0.226062984126984</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -8504,7 +8536,7 @@
         <v>0.227684444444444</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -8572,7 +8604,7 @@
         <v>0.26175291005291002</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -8640,7 +8672,7 @@
         <v>0.26755987301587197</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -8669,7 +8701,7 @@
         <v>0.33182754446553497</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -8698,7 +8730,7 @@
         <v>0.17106666666666601</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -8727,7 +8759,7 @@
         <v>0.25776888888888799</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -8756,7 +8788,7 @@
         <v>0.26755987301587197</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -8824,7 +8856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -8892,7 +8924,7 @@
         <v>4.8554497354496998E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -8960,7 +8992,7 @@
         <v>1.9317777777777701E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -9028,7 +9060,7 @@
         <v>2.3430582010581999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -9096,7 +9128,7 @@
         <v>1.8440634920634899E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -9164,7 +9196,7 @@
         <v>3.1680211640211599E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -9232,7 +9264,7 @@
         <v>3.7636825396825E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -9300,7 +9332,7 @@
         <v>2.7135238095238001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -9368,7 +9400,7 @@
         <v>4.5236039304610703E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -9397,7 +9429,7 @@
         <v>6.6125296616557E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -9426,7 +9458,7 @@
         <v>2.1919999999999999E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -9455,7 +9487,7 @@
         <v>4.1966666666666597E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -9484,7 +9516,7 @@
         <v>4.5236039304610703E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -9552,7 +9584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -9620,7 +9652,7 @@
         <v>2.34674973544973E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -9688,7 +9720,7 @@
         <v>1.6674962962962898E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -9756,7 +9788,7 @@
         <v>2.76662962962963E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -9824,7 +9856,7 @@
         <v>3.5556645502645499E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -9892,7 +9924,7 @@
         <v>1.9918476190476101E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -9960,7 +9992,7 @@
         <v>2.77221164021163E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -10028,7 +10060,7 @@
         <v>2.37222645502645E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -10096,7 +10128,7 @@
         <v>4.1415449735449701E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -10125,7 +10157,7 @@
         <v>7.3699174623340302E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -10154,7 +10186,7 @@
         <v>1.38438095238095E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -10183,7 +10215,7 @@
         <v>3.1792063492063399E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -10212,7 +10244,7 @@
         <v>4.1415449735449701E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -10280,7 +10312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -10348,7 +10380,7 @@
         <v>3.8133333333330001E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -10416,7 +10448,7 @@
         <v>5.7142857142857101E-5</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -10484,7 +10516,7 @@
         <v>2.4933333333333001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -10552,7 +10584,7 @@
         <v>4.9777777777770002E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -10620,7 +10652,7 @@
         <v>2.9047619047610002E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -10688,7 +10720,7 @@
         <v>1.5333333333333E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -10756,7 +10788,7 @@
         <v>6.3015873015870002E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -10824,7 +10856,7 @@
         <v>1.2463492063492E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -10853,7 +10885,7 @@
         <v>2.1445498749811001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -10882,7 +10914,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -10911,7 +10943,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -10940,32 +10972,32 @@
         <v>1.2463492063492E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B85" s="11" t="s">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A85" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D85" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E85" s="11" t="s">
+      <c r="E85" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="F85" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G85" s="11" t="s">
+      <c r="G85" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="H85" s="11" t="s">
+      <c r="H85" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I85" s="11" t="s">
+      <c r="I85" s="9" t="s">
         <v>95</v>
       </c>
       <c r="K85" t="str">
@@ -11021,7 +11053,7 @@
         <v>map_cut_10</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -11102,7 +11134,7 @@
         <v>0.4155209806694955</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -11183,7 +11215,7 @@
         <v>0.47794593745088798</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -11264,7 +11296,7 @@
         <v>0.46118890460474621</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -11345,7 +11377,7 @@
         <v>0.47417256011315417</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -11426,7 +11458,7 @@
         <v>0.44110639635392113</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -11507,7 +11539,7 @@
         <v>0.44461260411755471</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -11588,7 +11620,7 @@
         <v>0.46161873330190162</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -11669,7 +11701,7 @@
         <v>0.68479019330504476</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -11698,7 +11730,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -11727,7 +11759,7 @@
         <v>0.70960729180542281</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -11756,7 +11788,7 @@
         <v>0.71358751120038144</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -11785,7 +11817,7 @@
         <v>0.71728765166300479</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -11814,7 +11846,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -11843,7 +11875,7 @@
         <v>0.68306930693069312</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -11872,7 +11904,7 @@
         <v>0.68479019330504476</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -11901,7 +11933,7 @@
         <v>0.68536277648194477</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>17</v>
       </c>
@@ -11930,7 +11962,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -11959,7 +11991,7 @@
         <v>0.78613861386138617</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -11988,7 +12020,7 @@
         <v>0.79801980198019806</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -12026,66 +12058,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3A18D2-30FF-4570-A5C2-4E4FB86528D4}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="25" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9" t="s">
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9" t="s">
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
       <c r="B2" s="4" t="s">
         <v>83</v>
       </c>
@@ -12171,7 +12203,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -12247,24 +12279,24 @@
       <c r="Y3" s="3">
         <v>1.2133333333329999E-4</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3" s="12">
         <f>[3]Sheet1!B2</f>
         <v>0.33267326732673269</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="12">
         <f>[3]Sheet1!C2</f>
         <v>0.52475247524752477</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3" s="12">
         <f>[3]Sheet1!D2</f>
         <v>0.43433685881132428</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AC3" s="12">
         <f>[3]Sheet1!E2</f>
         <v>0.40422442244224421</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
@@ -12340,24 +12372,24 @@
       <c r="Y4" s="8">
         <v>1.5333333333333E-3</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4" s="12">
         <f>[3]Sheet1!B3</f>
         <v>0.37227722772277227</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4" s="12">
         <f>[3]Sheet1!C3</f>
         <v>0.52871287128712874</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="12">
         <f>[3]Sheet1!D3</f>
         <v>0.45956591316347828</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AC4" s="12">
         <f>[3]Sheet1!E3</f>
         <v>0.43623762376237629</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -12433,24 +12465,24 @@
       <c r="Y5" s="3">
         <v>5.7142857142857101E-5</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Z5" s="12">
         <f>[3]Sheet1!B4</f>
         <v>0.37029702970297029</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AA5" s="12">
         <f>[3]Sheet1!C4</f>
         <v>0.53861386138613865</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="12">
         <f>[3]Sheet1!D4</f>
         <v>0.45923120656909389</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AC5" s="12">
         <f>[3]Sheet1!E4</f>
         <v>0.43280528052805273</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
@@ -12526,24 +12558,24 @@
       <c r="Y6" s="3">
         <v>0</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z6" s="8">
         <f>[3]Sheet1!B5</f>
         <v>0.4138613861386139</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA6" s="8">
         <f>[3]Sheet1!C5</f>
         <v>0.56831683168316827</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB6" s="8">
         <f>[3]Sheet1!D5</f>
         <v>0.49393158719216779</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AC6" s="8">
         <f>[3]Sheet1!E5</f>
         <v>0.46937293729372931</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
@@ -12619,24 +12651,24 @@
       <c r="Y7" s="3">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="Z7" s="12">
         <f>[3]Sheet1!B6</f>
         <v>0.40396039603960399</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AA7" s="12">
         <f>[3]Sheet1!C6</f>
         <v>0.55841584158415847</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AB7" s="12">
         <f>[3]Sheet1!D6</f>
         <v>0.48832212190279489</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AC7" s="12">
         <f>[3]Sheet1!E6</f>
         <v>0.46478547854785479</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>71</v>
       </c>
@@ -12712,24 +12744,24 @@
       <c r="Y8" s="7">
         <v>2.2666666666666E-3</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="Z8" s="12">
         <f>[3]Sheet1!B7</f>
         <v>0.39801980198019798</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AA8" s="12">
         <f>[3]Sheet1!C7</f>
         <v>0.55049504950495054</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AB8" s="12">
         <f>[3]Sheet1!D7</f>
         <v>0.47867078650248568</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AC8" s="12">
         <f>[3]Sheet1!E7</f>
         <v>0.45485148514851481</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -12805,24 +12837,24 @@
       <c r="Y9" s="3">
         <v>0</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="Z9" s="12">
         <f>[3]Sheet1!B8</f>
         <v>0.39207920792079209</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AA9" s="12">
         <f>[3]Sheet1!C8</f>
         <v>0.56633663366336628</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AB9" s="12">
         <f>[3]Sheet1!D8</f>
         <v>0.4841750282211964</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AC9" s="12">
         <f>[3]Sheet1!E8</f>
         <v>0.45689768976897688</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -12898,24 +12930,24 @@
       <c r="Y10" s="3">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="Z10" s="7">
         <f>[3]Sheet1!B9</f>
         <v>0.598019801980198</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AA10" s="7">
         <f>[3]Sheet1!C9</f>
         <v>0.78613861386138617</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AB10" s="7">
         <f>[3]Sheet1!D9</f>
         <v>0.70960729180542281</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="AC10" s="7">
         <f>[3]Sheet1!E9</f>
         <v>0.68306930693069312</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -12953,75 +12985,87 @@
     <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10">
+    <cfRule type="top10" dxfId="27" priority="28" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C10">
+    <cfRule type="top10" dxfId="26" priority="27" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10">
+    <cfRule type="top10" dxfId="25" priority="26" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E10">
+    <cfRule type="top10" dxfId="24" priority="25" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F10">
     <cfRule type="top10" dxfId="23" priority="24" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C10">
+  <conditionalFormatting sqref="G3:G10">
     <cfRule type="top10" dxfId="22" priority="23" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D10">
+  <conditionalFormatting sqref="H3:H10">
     <cfRule type="top10" dxfId="21" priority="22" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E10">
+  <conditionalFormatting sqref="I3:I10">
     <cfRule type="top10" dxfId="20" priority="21" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F10">
+  <conditionalFormatting sqref="J3:J10">
     <cfRule type="top10" dxfId="19" priority="20" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G10">
+  <conditionalFormatting sqref="K3:K10">
     <cfRule type="top10" dxfId="18" priority="19" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H10">
+  <conditionalFormatting sqref="L3:L10">
     <cfRule type="top10" dxfId="17" priority="18" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I10">
+  <conditionalFormatting sqref="M3:M10">
     <cfRule type="top10" dxfId="16" priority="17" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="N3:N10">
     <cfRule type="top10" dxfId="15" priority="16" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K10">
+  <conditionalFormatting sqref="O3:O10">
     <cfRule type="top10" dxfId="14" priority="15" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L10">
+  <conditionalFormatting sqref="P3:P10">
     <cfRule type="top10" dxfId="13" priority="14" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M10">
+  <conditionalFormatting sqref="Q3:Q10">
     <cfRule type="top10" dxfId="12" priority="13" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N10">
+  <conditionalFormatting sqref="R3:R10">
     <cfRule type="top10" dxfId="11" priority="12" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O10">
+  <conditionalFormatting sqref="S3:S10">
     <cfRule type="top10" dxfId="10" priority="11" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P10">
+  <conditionalFormatting sqref="T3:T10">
     <cfRule type="top10" dxfId="9" priority="10" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q10">
+  <conditionalFormatting sqref="U3:U10">
     <cfRule type="top10" dxfId="8" priority="9" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R10">
+  <conditionalFormatting sqref="V3:V10">
     <cfRule type="top10" dxfId="7" priority="8" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S10">
+  <conditionalFormatting sqref="W3:W10">
     <cfRule type="top10" dxfId="6" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T10">
+  <conditionalFormatting sqref="X3:X10">
     <cfRule type="top10" dxfId="5" priority="6" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U10">
+  <conditionalFormatting sqref="Y3:Y10">
     <cfRule type="top10" dxfId="4" priority="5" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V10">
+  <conditionalFormatting sqref="Z3:Z10">
     <cfRule type="top10" dxfId="3" priority="4" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W10">
+  <conditionalFormatting sqref="AA3:AA10">
     <cfRule type="top10" dxfId="2" priority="3" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X10">
+  <conditionalFormatting sqref="AB3:AB10">
     <cfRule type="top10" dxfId="1" priority="2" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y10">
+  <conditionalFormatting sqref="AC3:AC10">
     <cfRule type="top10" dxfId="0" priority="1" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
results updated for bert-e2e-absa
</commit_message>
<xml_diff>
--- a/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
+++ b/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hfani/Github/fani-lab/LADy/main/output/2015SB12/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farinam\PycharmProjects\LADy\output\2015SB12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14C0CA5-B599-1B43-B728-DFCE5F18D4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75F6E8F-5EC4-4A12-B88C-5FA5CFB3D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21210" windowHeight="12990" activeTab="2" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="113">
   <si>
     <t>metric</t>
   </si>
@@ -332,6 +332,57 @@
   <si>
     <t>all.cat</t>
   </si>
+  <si>
+    <t>BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>arb_Arab.BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>deu_Latn.BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>fra_Latn.BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>pes_Arab.BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>zho_Hans.BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>spa_Latn.BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>pes_Arab.zho_Hans.deu_Latn.arb_Arab.fra_Latn.spa_Latn.BERT-E2E-ABSA.0.0</t>
+  </si>
+  <si>
+    <t>BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>arabic.BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>german.BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>french.BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>farsi.BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>chinese.BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>spanish.BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>all.BERT-E2E-ABSA</t>
+  </si>
+  <si>
+    <t>bert-e2e-absa</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +391,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,6 +420,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -468,8 +524,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2123,18 +2179,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DE02BE-45B7-4D8D-BCA0-35520325FAF3}">
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="F144" sqref="F144"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156:N179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2192,7 +2248,7 @@
         <v>0.21279999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2221,7 +2277,7 @@
         <v>8.89599999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2250,7 +2306,7 @@
         <v>5.2959999999999903E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2279,7 +2335,7 @@
         <v>1.0208E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2308,7 +2364,7 @@
         <v>0.152106666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2337,7 +2393,7 @@
         <v>0.29861333333333301</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2366,7 +2422,7 @@
         <v>0.35119999999999901</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2395,7 +2451,7 @@
         <v>0.59628571428571397</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2424,7 +2480,7 @@
         <v>0.21279999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2453,7 +2509,7 @@
         <v>0.25147113938973098</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2482,7 +2538,7 @@
         <v>0.27023987258530402</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2511,7 +2567,7 @@
         <v>0.33064506362917101</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2540,7 +2596,7 @@
         <v>0.152106666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2569,7 +2625,7 @@
         <v>0.21400177777777701</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2598,7 +2654,7 @@
         <v>0.22167585185185101</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2627,7 +2683,7 @@
         <v>0.23398065524836001</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2656,7 +2712,7 @@
         <v>0.21279999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2685,7 +2741,7 @@
         <v>0.38879999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2714,7 +2770,7 @@
         <v>0.46079999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2743,7 +2799,7 @@
         <v>0.74879999999999902</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2772,7 +2828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2801,7 +2857,7 @@
         <v>0.21920000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -2830,7 +2886,7 @@
         <v>7.9039999999999902E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2859,7 +2915,7 @@
         <v>4.65599999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2888,7 +2944,7 @@
         <v>1.0288E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -2917,7 +2973,7 @@
         <v>0.15122666666666601</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -2946,7 +3002,7 @@
         <v>0.247013333333333</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2975,7 +3031,7 @@
         <v>0.28414857142857097</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -3004,7 +3060,7 @@
         <v>0.59225714285714204</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -3033,7 +3089,7 @@
         <v>0.21920000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -3062,7 +3118,7 @@
         <v>0.22629866399950399</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -3091,7 +3147,7 @@
         <v>0.239501257872131</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3120,7 +3176,7 @@
         <v>0.31122066321356701</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -3149,7 +3205,7 @@
         <v>0.15122666666666601</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3178,7 +3234,7 @@
         <v>0.194193333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -3207,7 +3263,7 @@
         <v>0.19952719274376399</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -3236,7 +3292,7 @@
         <v>0.21316044074708701</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -3265,7 +3321,7 @@
         <v>0.21920000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -3294,7 +3350,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -3323,7 +3379,7 @@
         <v>0.40960000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -3352,7 +3408,7 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -3410,7 +3466,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -3439,7 +3495,7 @@
         <v>0.11359999999999899</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -3468,7 +3524,7 @@
         <v>6.7359999999999906E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3497,7 +3553,7 @@
         <v>9.8720000000000006E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -3526,7 +3582,7 @@
         <v>0.17106666666666601</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -3555,7 +3611,7 @@
         <v>0.374373333333333</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -3584,7 +3640,7 @@
         <v>0.43401523809523801</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -3613,7 +3669,7 @@
         <v>0.58357333333333306</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -3642,7 +3698,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3671,7 +3727,7 @@
         <v>0.31040362405493099</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -3700,7 +3756,7 @@
         <v>0.33182754446553497</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -3729,7 +3785,7 @@
         <v>0.37248576969911001</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -3758,7 +3814,7 @@
         <v>0.17106666666666601</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3787,7 +3843,7 @@
         <v>0.25776888888888799</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3816,7 +3872,7 @@
         <v>0.26755987301587197</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -3845,7 +3901,7 @@
         <v>0.277474289415583</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -3874,7 +3930,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -3903,7 +3959,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -3932,7 +3988,7 @@
         <v>0.56640000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -3961,7 +4017,7 @@
         <v>0.74079999999999901</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -3990,7 +4046,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -4019,7 +4075,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -4048,7 +4104,7 @@
         <v>2.656E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -4077,7 +4133,7 @@
         <v>1.7440000000000001E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -4106,7 +4162,7 @@
         <v>6.0480000000000004E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -4135,7 +4191,7 @@
         <v>2.1919999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -4164,7 +4220,7 @@
         <v>7.5653333333333295E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -4193,7 +4249,7 @@
         <v>9.7641904761904694E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -4222,7 +4278,7 @@
         <v>0.35544761904761901</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -4251,7 +4307,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -4280,7 +4336,7 @@
         <v>5.8043532868121799E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -4309,7 +4365,7 @@
         <v>6.6125296616557E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -4338,7 +4394,7 @@
         <v>0.121637011287014</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -4367,7 +4423,7 @@
         <v>2.1919999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4396,7 +4452,7 @@
         <v>4.1966666666666597E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -4425,7 +4481,7 @@
         <v>4.5236039304610703E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -4454,7 +4510,7 @@
         <v>5.3798705533092003E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -4483,7 +4539,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -4512,7 +4568,7 @@
         <v>0.12640000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -4541,7 +4597,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>20</v>
       </c>
@@ -4570,7 +4626,7 @@
         <v>0.50560000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -4599,7 +4655,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -4628,7 +4684,7 @@
         <v>2.24E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -4657,7 +4713,7 @@
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -4686,7 +4742,7 @@
         <v>2.5919999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>4</v>
       </c>
@@ -4715,7 +4771,7 @@
         <v>7.9360000000000003E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -4744,7 +4800,7 @@
         <v>1.38438095238095E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -4773,7 +4829,7 @@
         <v>7.3100952380952294E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -4802,7 +4858,7 @@
         <v>0.14519619047619001</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -4831,7 +4887,7 @@
         <v>0.45667238095238</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -4860,7 +4916,7 @@
         <v>2.24E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4889,7 +4945,7 @@
         <v>4.78374663687973E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -4918,7 +4974,7 @@
         <v>7.3699174623340302E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -4947,7 +5003,7 @@
         <v>0.14382513812276401</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -4976,7 +5032,7 @@
         <v>1.38438095238095E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -5005,7 +5061,7 @@
         <v>3.1792063492063399E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -5034,7 +5090,7 @@
         <v>4.1415449735449701E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -5063,7 +5119,7 @@
         <v>5.3546239917164999E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>17</v>
       </c>
@@ -5092,7 +5148,7 @@
         <v>2.24E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -5121,7 +5177,7 @@
         <v>0.1216</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>19</v>
       </c>
@@ -5150,7 +5206,7 @@
         <v>0.23680000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>20</v>
       </c>
@@ -5179,7 +5235,7 @@
         <v>0.62080000000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -5208,7 +5264,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -5237,7 +5293,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -5266,7 +5322,7 @@
         <v>3.2000000000000003E-4</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>3</v>
       </c>
@@ -5295,7 +5351,7 @@
         <v>6.4000000000000005E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>4</v>
       </c>
@@ -5324,7 +5380,7 @@
         <v>9.6000000000000002E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -5353,7 +5409,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -5382,7 +5438,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -5411,7 +5467,7 @@
         <v>4.1066666666665997E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -5440,7 +5496,7 @@
         <v>4.4799999999999996E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -5469,7 +5525,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -5498,7 +5554,7 @@
         <v>9.8103550842470002E-4</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -5527,7 +5583,7 @@
         <v>2.1445498749811001E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>12</v>
       </c>
@@ -5556,7 +5612,7 @@
         <v>2.3114484496906998E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -5585,7 +5641,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>14</v>
       </c>
@@ -5614,7 +5670,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -5643,7 +5699,7 @@
         <v>1.2463492063492E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>16</v>
       </c>
@@ -5672,7 +5728,7 @@
         <v>1.2744973544973001E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -5701,7 +5757,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>18</v>
       </c>
@@ -5730,7 +5786,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>19</v>
       </c>
@@ -5759,7 +5815,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>20</v>
       </c>
@@ -5788,7 +5844,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
         <f>[1]Sheet1!A1</f>
         <v>metric</v>
@@ -5826,7 +5882,7 @@
         <v>pes_Arab.zho_Hans.deu_Latn.arb_Arab.fra_Latn.spa_Latn.cat.0.0</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f>[1]Sheet1!A2</f>
         <v>P_1</v>
@@ -5864,7 +5920,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
         <f>[1]Sheet1!A3</f>
         <v>P_5</v>
@@ -5902,7 +5958,7 @@
         <v>0.1572277227722769</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
         <f>[1]Sheet1!A4</f>
         <v>P_10</v>
@@ -5940,7 +5996,7 @@
         <v>7.9801980198019595E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
         <f>[1]Sheet1!A5</f>
         <v>P_100</v>
@@ -5978,7 +6034,7 @@
         <v>8.1782178217821005E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
         <f>[1]Sheet1!A6</f>
         <v>recall_1</v>
@@ -6016,7 +6072,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
         <f>[1]Sheet1!A7</f>
         <v>recall_5</v>
@@ -6054,7 +6110,7 @@
         <v>0.78613861386138617</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
         <f>[1]Sheet1!A8</f>
         <v>recall_10</v>
@@ -6092,7 +6148,7 @@
         <v>0.79801980198019806</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
         <f>[1]Sheet1!A9</f>
         <v>recall_100</v>
@@ -6130,7 +6186,7 @@
         <v>0.81782178217821788</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
         <f>[1]Sheet1!A10</f>
         <v>ndcg_cut_1</v>
@@ -6168,7 +6224,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
         <f>[1]Sheet1!A11</f>
         <v>ndcg_cut_5</v>
@@ -6206,7 +6262,7 @@
         <v>0.70960729180542281</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
         <f>[1]Sheet1!A12</f>
         <v>ndcg_cut_10</v>
@@ -6244,7 +6300,7 @@
         <v>0.71358751120038144</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f>[1]Sheet1!A13</f>
         <v>ndcg_cut_100</v>
@@ -6282,7 +6338,7 @@
         <v>0.71728765166300479</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f>[1]Sheet1!A14</f>
         <v>map_cut_1</v>
@@ -6320,7 +6376,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f>[1]Sheet1!A15</f>
         <v>map_cut_5</v>
@@ -6358,7 +6414,7 @@
         <v>0.68306930693069312</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f>[1]Sheet1!A16</f>
         <v>map_cut_10</v>
@@ -6396,7 +6452,7 @@
         <v>0.68479019330504476</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f>[1]Sheet1!A17</f>
         <v>map_cut_100</v>
@@ -6434,7 +6490,7 @@
         <v>0.68536277648194477</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f>[1]Sheet1!A18</f>
         <v>success_1</v>
@@ -6472,7 +6528,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f>[1]Sheet1!A19</f>
         <v>success_5</v>
@@ -6510,7 +6566,7 @@
         <v>0.78613861386138617</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f>[1]Sheet1!A20</f>
         <v>success_10</v>
@@ -6548,7 +6604,7 @@
         <v>0.79801980198019806</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f>[1]Sheet1!A21</f>
         <v>success_100</v>
@@ -6584,6 +6640,615 @@
       <c r="I153">
         <f>[1]Sheet1!I21</f>
         <v>0.81782178217821788</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C156" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D156" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E156" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F156" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G156" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H156" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I156" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>0.7</v>
+      </c>
+      <c r="C157">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="D157">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="E157">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="F157">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="G157">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="H157">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="I157">
+        <v>0.66129032258064513</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>2</v>
+      </c>
+      <c r="B158">
+        <v>0.25193548387096792</v>
+      </c>
+      <c r="C158">
+        <v>0.25161290322580637</v>
+      </c>
+      <c r="D158">
+        <v>0.25161290322580648</v>
+      </c>
+      <c r="E158">
+        <v>0.25645161290322582</v>
+      </c>
+      <c r="F158">
+        <v>0.24580645161290329</v>
+      </c>
+      <c r="G158">
+        <v>0.25322580645161291</v>
+      </c>
+      <c r="H158">
+        <v>0.25903225806451619</v>
+      </c>
+      <c r="I158">
+        <v>0.26032258064516128</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>3</v>
+      </c>
+      <c r="B159">
+        <v>0.14580645161290329</v>
+      </c>
+      <c r="C159">
+        <v>0.14532258064516129</v>
+      </c>
+      <c r="D159">
+        <v>0.14741935483870969</v>
+      </c>
+      <c r="E159">
+        <v>0.14887096774193551</v>
+      </c>
+      <c r="F159">
+        <v>0.1438709677419355</v>
+      </c>
+      <c r="G159">
+        <v>0.14790322580645171</v>
+      </c>
+      <c r="H159">
+        <v>0.14725806451612911</v>
+      </c>
+      <c r="I159">
+        <v>0.14838709677419351</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>4</v>
+      </c>
+      <c r="B160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="C160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="D160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="E160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="F160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="G160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="H160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="I160">
+        <v>1.6451612903225811E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161">
+        <v>0.46804723502304152</v>
+      </c>
+      <c r="C161">
+        <v>0.4527784178187404</v>
+      </c>
+      <c r="D161">
+        <v>0.45534562211981572</v>
+      </c>
+      <c r="E161">
+        <v>0.44365207373271892</v>
+      </c>
+      <c r="F161">
+        <v>0.45780529953917048</v>
+      </c>
+      <c r="G161">
+        <v>0.45048003072196618</v>
+      </c>
+      <c r="H161">
+        <v>0.44941820276497713</v>
+      </c>
+      <c r="I161">
+        <v>0.44820852534562211</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>6</v>
+      </c>
+      <c r="B162">
+        <v>0.68967741935483873</v>
+      </c>
+      <c r="C162">
+        <v>0.6897964669738863</v>
+      </c>
+      <c r="D162">
+        <v>0.69269009216589861</v>
+      </c>
+      <c r="E162">
+        <v>0.70302611367127488</v>
+      </c>
+      <c r="F162">
+        <v>0.67068548387096771</v>
+      </c>
+      <c r="G162">
+        <v>0.69278225806451621</v>
+      </c>
+      <c r="H162">
+        <v>0.7098540706605222</v>
+      </c>
+      <c r="I162">
+        <v>0.71817012288786475</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163">
+        <v>0.76975806451612905</v>
+      </c>
+      <c r="C163">
+        <v>0.76813172043010758</v>
+      </c>
+      <c r="D163">
+        <v>0.7714112903225806</v>
+      </c>
+      <c r="E163">
+        <v>0.78104838709677415</v>
+      </c>
+      <c r="F163">
+        <v>0.7577956989247312</v>
+      </c>
+      <c r="G163">
+        <v>0.77989247311827958</v>
+      </c>
+      <c r="H163">
+        <v>0.77775537634408598</v>
+      </c>
+      <c r="I163">
+        <v>0.77895161290322579</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="C164">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="D164">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="E164">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="F164">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="G164">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="H164">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="I164">
+        <v>0.83239247311827957</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>9</v>
+      </c>
+      <c r="B165">
+        <v>0.7</v>
+      </c>
+      <c r="C165">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="D165">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="E165">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="F165">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="G165">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="H165">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="I165">
+        <v>0.66129032258064513</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>10</v>
+      </c>
+      <c r="B166">
+        <v>0.67569639194713516</v>
+      </c>
+      <c r="C166">
+        <v>0.6671126897849724</v>
+      </c>
+      <c r="D166">
+        <v>0.6721386619249281</v>
+      </c>
+      <c r="E166">
+        <v>0.67340833792219734</v>
+      </c>
+      <c r="F166">
+        <v>0.66083863314591729</v>
+      </c>
+      <c r="G166">
+        <v>0.66991932689621814</v>
+      </c>
+      <c r="H166">
+        <v>0.6769417849229501</v>
+      </c>
+      <c r="I166">
+        <v>0.68226776500892794</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>11</v>
+      </c>
+      <c r="B167">
+        <v>0.70512505515545087</v>
+      </c>
+      <c r="C167">
+        <v>0.69625897127709246</v>
+      </c>
+      <c r="D167">
+        <v>0.70245263163347793</v>
+      </c>
+      <c r="E167">
+        <v>0.70251917046246315</v>
+      </c>
+      <c r="F167">
+        <v>0.69255296422884216</v>
+      </c>
+      <c r="G167">
+        <v>0.70228681512738456</v>
+      </c>
+      <c r="H167">
+        <v>0.70225044431933914</v>
+      </c>
+      <c r="I167">
+        <v>0.70517385335412308</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>12</v>
+      </c>
+      <c r="B168">
+        <v>0.72665782150875668</v>
+      </c>
+      <c r="C168">
+        <v>0.71824283713922044</v>
+      </c>
+      <c r="D168">
+        <v>0.72267288339285729</v>
+      </c>
+      <c r="E168">
+        <v>0.71984080202643208</v>
+      </c>
+      <c r="F168">
+        <v>0.71720552563622242</v>
+      </c>
+      <c r="G168">
+        <v>0.72050050341331839</v>
+      </c>
+      <c r="H168">
+        <v>0.72100281284068302</v>
+      </c>
+      <c r="I168">
+        <v>0.72358625314130742</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>13</v>
+      </c>
+      <c r="B169">
+        <v>0.46804723502304152</v>
+      </c>
+      <c r="C169">
+        <v>0.4527784178187404</v>
+      </c>
+      <c r="D169">
+        <v>0.45534562211981572</v>
+      </c>
+      <c r="E169">
+        <v>0.44365207373271892</v>
+      </c>
+      <c r="F169">
+        <v>0.45780529953917048</v>
+      </c>
+      <c r="G169">
+        <v>0.45048003072196618</v>
+      </c>
+      <c r="H169">
+        <v>0.44941820276497713</v>
+      </c>
+      <c r="I169">
+        <v>0.44820852534562211</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>14</v>
+      </c>
+      <c r="B170">
+        <v>0.6246427611367128</v>
+      </c>
+      <c r="C170">
+        <v>0.61343362775217614</v>
+      </c>
+      <c r="D170">
+        <v>0.61857338069636447</v>
+      </c>
+      <c r="E170">
+        <v>0.61805619559651814</v>
+      </c>
+      <c r="F170">
+        <v>0.61012544802867386</v>
+      </c>
+      <c r="G170">
+        <v>0.61723790322580652</v>
+      </c>
+      <c r="H170">
+        <v>0.62034399001536089</v>
+      </c>
+      <c r="I170">
+        <v>0.62366481054787504</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>15</v>
+      </c>
+      <c r="B171">
+        <v>0.64693134951113063</v>
+      </c>
+      <c r="C171">
+        <v>0.63604794973544976</v>
+      </c>
+      <c r="D171">
+        <v>0.64192677474215487</v>
+      </c>
+      <c r="E171">
+        <v>0.64041688001365427</v>
+      </c>
+      <c r="F171">
+        <v>0.63291546278009414</v>
+      </c>
+      <c r="G171">
+        <v>0.64048713822446535</v>
+      </c>
+      <c r="H171">
+        <v>0.64072502773510831</v>
+      </c>
+      <c r="I171">
+        <v>0.64238610013898023</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>16</v>
+      </c>
+      <c r="B172">
+        <v>0.65739190523195057</v>
+      </c>
+      <c r="C172">
+        <v>0.64684139733675339</v>
+      </c>
+      <c r="D172">
+        <v>0.65182901437739937</v>
+      </c>
+      <c r="E172">
+        <v>0.64930170554740796</v>
+      </c>
+      <c r="F172">
+        <v>0.6446229701549766</v>
+      </c>
+      <c r="G172">
+        <v>0.64975592434607266</v>
+      </c>
+      <c r="H172">
+        <v>0.6503511757401097</v>
+      </c>
+      <c r="I172">
+        <v>0.65218680465199008</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>17</v>
+      </c>
+      <c r="B173">
+        <v>0.7</v>
+      </c>
+      <c r="C173">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="D173">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="E173">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="F173">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="G173">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="H173">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="I173">
+        <v>0.66129032258064513</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>18</v>
+      </c>
+      <c r="B174">
+        <v>0.80806451612903218</v>
+      </c>
+      <c r="C174">
+        <v>0.81612903225806455</v>
+      </c>
+      <c r="D174">
+        <v>0.81935483870967762</v>
+      </c>
+      <c r="E174">
+        <v>0.82258064516129037</v>
+      </c>
+      <c r="F174">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="G174">
+        <v>0.81774193548387097</v>
+      </c>
+      <c r="H174">
+        <v>0.82741935483870965</v>
+      </c>
+      <c r="I174">
+        <v>0.84193548387096784</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>19</v>
+      </c>
+      <c r="B175">
+        <v>0.85967741935483866</v>
+      </c>
+      <c r="C175">
+        <v>0.85806451612903234</v>
+      </c>
+      <c r="D175">
+        <v>0.86290322580645162</v>
+      </c>
+      <c r="E175">
+        <v>0.87096774193548376</v>
+      </c>
+      <c r="F175">
+        <v>0.85483870967741937</v>
+      </c>
+      <c r="G175">
+        <v>0.87096774193548376</v>
+      </c>
+      <c r="H175">
+        <v>0.86774193548387091</v>
+      </c>
+      <c r="I175">
+        <v>0.87096774193548376</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>20</v>
+      </c>
+      <c r="B176">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="C176">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="D176">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="E176">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="F176">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="G176">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="H176">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="I176">
+        <v>0.88709677419354838</v>
       </c>
     </row>
   </sheetData>
@@ -6593,18 +7258,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8DF60C-3A99-4B9F-820E-01296226828F}">
-  <dimension ref="A1:W105"/>
+  <dimension ref="A1:AE128"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView topLeftCell="F105" workbookViewId="0">
+      <selection activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6672,7 +7337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6740,7 +7405,7 @@
         <v>0.21275286772486701</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6808,7 +7473,7 @@
         <v>0.192248296296296</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6876,7 +7541,7 @@
         <v>0.200167809523809</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -6944,7 +7609,7 @@
         <v>0.22157174603174501</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -7012,7 +7677,7 @@
         <v>0.198939978835978</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -7080,7 +7745,7 @@
         <v>0.20257053665910801</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -7148,7 +7813,7 @@
         <v>0.21551279365079301</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -7216,7 +7881,7 @@
         <v>0.22167585185185101</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -7245,7 +7910,7 @@
         <v>0.27023987258530402</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -7274,7 +7939,7 @@
         <v>0.152106666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -7303,7 +7968,7 @@
         <v>0.21400177777777701</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -7332,7 +7997,7 @@
         <v>0.22167585185185101</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -7400,7 +8065,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -7468,7 +8133,7 @@
         <v>4.4582222222222197E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -7536,7 +8201,7 @@
         <v>4.8447830687830602E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -7604,7 +8269,7 @@
         <v>5.1454285714285702E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -7672,7 +8337,7 @@
         <v>6.1332275132275099E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -7740,7 +8405,7 @@
         <v>6.2814126984126903E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -7808,7 +8473,7 @@
         <v>5.6631746031745998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -7876,7 +8541,7 @@
         <v>3.8382751322751298E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -7944,7 +8609,7 @@
         <v>0.19952719274376399</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -7973,7 +8638,7 @@
         <v>0.239501257872131</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -8002,7 +8667,7 @@
         <v>0.15122666666666601</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -8031,7 +8696,7 @@
         <v>0.194193333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -8060,7 +8725,7 @@
         <v>0.19952719274376399</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -8128,7 +8793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -8196,7 +8861,7 @@
         <v>0.25492650793650701</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -8264,7 +8929,7 @@
         <v>0.24628016931216901</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -8332,7 +8997,7 @@
         <v>0.26086635978835898</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -8400,7 +9065,7 @@
         <v>0.26959068783068701</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -8468,7 +9133,7 @@
         <v>0.226062984126984</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -8536,7 +9201,7 @@
         <v>0.227684444444444</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -8604,7 +9269,7 @@
         <v>0.26175291005291002</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -8672,7 +9337,7 @@
         <v>0.26755987301587197</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -8701,7 +9366,7 @@
         <v>0.33182754446553497</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -8730,7 +9395,7 @@
         <v>0.17106666666666601</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -8759,7 +9424,7 @@
         <v>0.25776888888888799</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -8788,7 +9453,7 @@
         <v>0.26755987301587197</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -8856,7 +9521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -8924,7 +9589,7 @@
         <v>4.8554497354496998E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -8992,7 +9657,7 @@
         <v>1.9317777777777701E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -9060,7 +9725,7 @@
         <v>2.3430582010581999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -9128,7 +9793,7 @@
         <v>1.8440634920634899E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -9196,7 +9861,7 @@
         <v>3.1680211640211599E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -9264,7 +9929,7 @@
         <v>3.7636825396825E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -9332,7 +9997,7 @@
         <v>2.7135238095238001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -9400,7 +10065,7 @@
         <v>4.5236039304610703E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -9429,7 +10094,7 @@
         <v>6.6125296616557E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -9458,7 +10123,7 @@
         <v>2.1919999999999999E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -9487,7 +10152,7 @@
         <v>4.1966666666666597E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -9516,7 +10181,7 @@
         <v>4.5236039304610703E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -9584,7 +10249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -9652,7 +10317,7 @@
         <v>2.34674973544973E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -9720,7 +10385,7 @@
         <v>1.6674962962962898E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -9788,7 +10453,7 @@
         <v>2.76662962962963E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -9856,7 +10521,7 @@
         <v>3.5556645502645499E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -9924,7 +10589,7 @@
         <v>1.9918476190476101E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -9992,7 +10657,7 @@
         <v>2.77221164021163E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -10060,7 +10725,7 @@
         <v>2.37222645502645E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -10128,7 +10793,7 @@
         <v>4.1415449735449701E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -10157,7 +10822,7 @@
         <v>7.3699174623340302E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -10186,7 +10851,7 @@
         <v>1.38438095238095E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -10215,7 +10880,7 @@
         <v>3.1792063492063399E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -10244,7 +10909,7 @@
         <v>4.1415449735449701E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -10312,7 +10977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -10380,7 +11045,7 @@
         <v>3.8133333333330001E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -10448,7 +11113,7 @@
         <v>5.7142857142857101E-5</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -10516,7 +11181,7 @@
         <v>2.4933333333333001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -10584,7 +11249,7 @@
         <v>4.9777777777770002E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -10652,7 +11317,7 @@
         <v>2.9047619047610002E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -10720,7 +11385,7 @@
         <v>1.5333333333333E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -10788,7 +11453,7 @@
         <v>6.3015873015870002E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -10856,7 +11521,7 @@
         <v>1.2463492063492E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -10885,7 +11550,7 @@
         <v>2.1445498749811001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -10914,7 +11579,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -10943,7 +11608,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -10972,7 +11637,7 @@
         <v>1.2463492063492E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>0</v>
       </c>
@@ -11053,7 +11718,7 @@
         <v>map_cut_10</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -11134,7 +11799,7 @@
         <v>0.4155209806694955</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -11215,7 +11880,7 @@
         <v>0.47794593745088798</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -11296,7 +11961,7 @@
         <v>0.46118890460474621</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -11377,7 +12042,7 @@
         <v>0.47417256011315417</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -11458,7 +12123,7 @@
         <v>0.44110639635392113</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -11539,7 +12204,7 @@
         <v>0.44461260411755471</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -11620,7 +12285,7 @@
         <v>0.46161873330190162</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -11701,7 +12366,7 @@
         <v>0.68479019330504476</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -11730,7 +12395,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -11759,7 +12424,7 @@
         <v>0.70960729180542281</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -11788,7 +12453,7 @@
         <v>0.71358751120038144</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -11817,7 +12482,7 @@
         <v>0.71728765166300479</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -11846,7 +12511,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -11875,7 +12540,7 @@
         <v>0.68306930693069312</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -11904,7 +12569,7 @@
         <v>0.68479019330504476</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -11933,7 +12598,7 @@
         <v>0.68536277648194477</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>17</v>
       </c>
@@ -11962,7 +12627,7 @@
         <v>0.598019801980198</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -11991,7 +12656,7 @@
         <v>0.78613861386138617</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -12020,7 +12685,7 @@
         <v>0.79801980198019806</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -12047,6 +12712,1182 @@
       </c>
       <c r="I105">
         <v>0.81782178217821788</v>
+      </c>
+    </row>
+    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A108" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H108" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I108" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K108" t="s">
+        <v>0</v>
+      </c>
+      <c r="L108" t="s">
+        <v>1</v>
+      </c>
+      <c r="M108" t="s">
+        <v>2</v>
+      </c>
+      <c r="N108" t="s">
+        <v>3</v>
+      </c>
+      <c r="O108" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>6</v>
+      </c>
+      <c r="R108" t="s">
+        <v>7</v>
+      </c>
+      <c r="S108" t="s">
+        <v>8</v>
+      </c>
+      <c r="T108" t="s">
+        <v>9</v>
+      </c>
+      <c r="U108" t="s">
+        <v>10</v>
+      </c>
+      <c r="V108" t="s">
+        <v>11</v>
+      </c>
+      <c r="W108" t="s">
+        <v>12</v>
+      </c>
+      <c r="X108" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y108" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z108" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB108" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC108" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD108" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE108" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>0.7</v>
+      </c>
+      <c r="C109">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="D109">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="E109">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="F109">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="G109">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="H109">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="I109">
+        <v>0.66129032258064513</v>
+      </c>
+      <c r="K109" t="s">
+        <v>104</v>
+      </c>
+      <c r="L109">
+        <v>0.7</v>
+      </c>
+      <c r="M109">
+        <v>0.25193548387096792</v>
+      </c>
+      <c r="N109">
+        <v>0.14580645161290329</v>
+      </c>
+      <c r="O109">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P109">
+        <v>0.46804723502304152</v>
+      </c>
+      <c r="Q109">
+        <v>0.68967741935483873</v>
+      </c>
+      <c r="R109">
+        <v>0.76975806451612905</v>
+      </c>
+      <c r="S109">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T109">
+        <v>0.7</v>
+      </c>
+      <c r="U109">
+        <v>0.67569639194713516</v>
+      </c>
+      <c r="V109">
+        <v>0.70512505515545087</v>
+      </c>
+      <c r="W109">
+        <v>0.72665782150875668</v>
+      </c>
+      <c r="X109">
+        <v>0.46804723502304152</v>
+      </c>
+      <c r="Y109">
+        <v>0.6246427611367128</v>
+      </c>
+      <c r="Z109">
+        <v>0.64693134951113063</v>
+      </c>
+      <c r="AA109">
+        <v>0.65739190523195057</v>
+      </c>
+      <c r="AB109">
+        <v>0.7</v>
+      </c>
+      <c r="AC109">
+        <v>0.80806451612903218</v>
+      </c>
+      <c r="AD109">
+        <v>0.85967741935483866</v>
+      </c>
+      <c r="AE109">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110">
+        <v>0.25193548387096792</v>
+      </c>
+      <c r="C110">
+        <v>0.25161290322580637</v>
+      </c>
+      <c r="D110">
+        <v>0.25161290322580648</v>
+      </c>
+      <c r="E110">
+        <v>0.25645161290322582</v>
+      </c>
+      <c r="F110">
+        <v>0.24580645161290329</v>
+      </c>
+      <c r="G110">
+        <v>0.25322580645161291</v>
+      </c>
+      <c r="H110">
+        <v>0.25903225806451619</v>
+      </c>
+      <c r="I110">
+        <v>0.26032258064516128</v>
+      </c>
+      <c r="K110" t="s">
+        <v>105</v>
+      </c>
+      <c r="L110">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="M110">
+        <v>0.25161290322580637</v>
+      </c>
+      <c r="N110">
+        <v>0.14532258064516129</v>
+      </c>
+      <c r="O110">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P110">
+        <v>0.4527784178187404</v>
+      </c>
+      <c r="Q110">
+        <v>0.6897964669738863</v>
+      </c>
+      <c r="R110">
+        <v>0.76813172043010758</v>
+      </c>
+      <c r="S110">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T110">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="U110">
+        <v>0.6671126897849724</v>
+      </c>
+      <c r="V110">
+        <v>0.69625897127709246</v>
+      </c>
+      <c r="W110">
+        <v>0.71824283713922044</v>
+      </c>
+      <c r="X110">
+        <v>0.4527784178187404</v>
+      </c>
+      <c r="Y110">
+        <v>0.61343362775217614</v>
+      </c>
+      <c r="Z110">
+        <v>0.63604794973544976</v>
+      </c>
+      <c r="AA110">
+        <v>0.64684139733675339</v>
+      </c>
+      <c r="AB110">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="AC110">
+        <v>0.81612903225806455</v>
+      </c>
+      <c r="AD110">
+        <v>0.85806451612903234</v>
+      </c>
+      <c r="AE110">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111">
+        <v>0.14580645161290329</v>
+      </c>
+      <c r="C111">
+        <v>0.14532258064516129</v>
+      </c>
+      <c r="D111">
+        <v>0.14741935483870969</v>
+      </c>
+      <c r="E111">
+        <v>0.14887096774193551</v>
+      </c>
+      <c r="F111">
+        <v>0.1438709677419355</v>
+      </c>
+      <c r="G111">
+        <v>0.14790322580645171</v>
+      </c>
+      <c r="H111">
+        <v>0.14725806451612911</v>
+      </c>
+      <c r="I111">
+        <v>0.14838709677419351</v>
+      </c>
+      <c r="K111" t="s">
+        <v>106</v>
+      </c>
+      <c r="L111">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="M111">
+        <v>0.25161290322580648</v>
+      </c>
+      <c r="N111">
+        <v>0.14741935483870969</v>
+      </c>
+      <c r="O111">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P111">
+        <v>0.45534562211981572</v>
+      </c>
+      <c r="Q111">
+        <v>0.69269009216589861</v>
+      </c>
+      <c r="R111">
+        <v>0.7714112903225806</v>
+      </c>
+      <c r="S111">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T111">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="U111">
+        <v>0.6721386619249281</v>
+      </c>
+      <c r="V111">
+        <v>0.70245263163347793</v>
+      </c>
+      <c r="W111">
+        <v>0.72267288339285729</v>
+      </c>
+      <c r="X111">
+        <v>0.45534562211981572</v>
+      </c>
+      <c r="Y111">
+        <v>0.61857338069636447</v>
+      </c>
+      <c r="Z111">
+        <v>0.64192677474215487</v>
+      </c>
+      <c r="AA111">
+        <v>0.65182901437739937</v>
+      </c>
+      <c r="AB111">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="AC111">
+        <v>0.81935483870967762</v>
+      </c>
+      <c r="AD111">
+        <v>0.86290322580645162</v>
+      </c>
+      <c r="AE111">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="C112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="D112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="E112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="F112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="G112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="H112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="I112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="K112" t="s">
+        <v>107</v>
+      </c>
+      <c r="L112">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="M112">
+        <v>0.25645161290322582</v>
+      </c>
+      <c r="N112">
+        <v>0.14887096774193551</v>
+      </c>
+      <c r="O112">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P112">
+        <v>0.44365207373271892</v>
+      </c>
+      <c r="Q112">
+        <v>0.70302611367127488</v>
+      </c>
+      <c r="R112">
+        <v>0.78104838709677415</v>
+      </c>
+      <c r="S112">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T112">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="U112">
+        <v>0.67340833792219734</v>
+      </c>
+      <c r="V112">
+        <v>0.70251917046246315</v>
+      </c>
+      <c r="W112">
+        <v>0.71984080202643208</v>
+      </c>
+      <c r="X112">
+        <v>0.44365207373271892</v>
+      </c>
+      <c r="Y112">
+        <v>0.61805619559651814</v>
+      </c>
+      <c r="Z112">
+        <v>0.64041688001365427</v>
+      </c>
+      <c r="AA112">
+        <v>0.64930170554740796</v>
+      </c>
+      <c r="AB112">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="AC112">
+        <v>0.82258064516129037</v>
+      </c>
+      <c r="AD112">
+        <v>0.87096774193548376</v>
+      </c>
+      <c r="AE112">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="113" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113">
+        <v>0.46804723502304152</v>
+      </c>
+      <c r="C113">
+        <v>0.4527784178187404</v>
+      </c>
+      <c r="D113">
+        <v>0.45534562211981572</v>
+      </c>
+      <c r="E113">
+        <v>0.44365207373271892</v>
+      </c>
+      <c r="F113">
+        <v>0.45780529953917048</v>
+      </c>
+      <c r="G113">
+        <v>0.45048003072196618</v>
+      </c>
+      <c r="H113">
+        <v>0.44941820276497713</v>
+      </c>
+      <c r="I113">
+        <v>0.44820852534562211</v>
+      </c>
+      <c r="K113" t="s">
+        <v>108</v>
+      </c>
+      <c r="L113">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="M113">
+        <v>0.24580645161290329</v>
+      </c>
+      <c r="N113">
+        <v>0.1438709677419355</v>
+      </c>
+      <c r="O113">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P113">
+        <v>0.45780529953917048</v>
+      </c>
+      <c r="Q113">
+        <v>0.67068548387096771</v>
+      </c>
+      <c r="R113">
+        <v>0.7577956989247312</v>
+      </c>
+      <c r="S113">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T113">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="U113">
+        <v>0.66083863314591729</v>
+      </c>
+      <c r="V113">
+        <v>0.69255296422884216</v>
+      </c>
+      <c r="W113">
+        <v>0.71720552563622242</v>
+      </c>
+      <c r="X113">
+        <v>0.45780529953917048</v>
+      </c>
+      <c r="Y113">
+        <v>0.61012544802867386</v>
+      </c>
+      <c r="Z113">
+        <v>0.63291546278009414</v>
+      </c>
+      <c r="AA113">
+        <v>0.6446229701549766</v>
+      </c>
+      <c r="AB113">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="AC113">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="AD113">
+        <v>0.85483870967741937</v>
+      </c>
+      <c r="AE113">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114">
+        <v>0.68967741935483873</v>
+      </c>
+      <c r="C114">
+        <v>0.6897964669738863</v>
+      </c>
+      <c r="D114">
+        <v>0.69269009216589861</v>
+      </c>
+      <c r="E114">
+        <v>0.70302611367127488</v>
+      </c>
+      <c r="F114">
+        <v>0.67068548387096771</v>
+      </c>
+      <c r="G114">
+        <v>0.69278225806451621</v>
+      </c>
+      <c r="H114">
+        <v>0.7098540706605222</v>
+      </c>
+      <c r="I114">
+        <v>0.71817012288786475</v>
+      </c>
+      <c r="K114" t="s">
+        <v>109</v>
+      </c>
+      <c r="L114">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="M114">
+        <v>0.25322580645161291</v>
+      </c>
+      <c r="N114">
+        <v>0.14790322580645171</v>
+      </c>
+      <c r="O114">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P114">
+        <v>0.45048003072196618</v>
+      </c>
+      <c r="Q114">
+        <v>0.69278225806451621</v>
+      </c>
+      <c r="R114">
+        <v>0.77989247311827958</v>
+      </c>
+      <c r="S114">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T114">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="U114">
+        <v>0.66991932689621814</v>
+      </c>
+      <c r="V114">
+        <v>0.70228681512738456</v>
+      </c>
+      <c r="W114">
+        <v>0.72050050341331839</v>
+      </c>
+      <c r="X114">
+        <v>0.45048003072196618</v>
+      </c>
+      <c r="Y114">
+        <v>0.61723790322580652</v>
+      </c>
+      <c r="Z114">
+        <v>0.64048713822446535</v>
+      </c>
+      <c r="AA114">
+        <v>0.64975592434607266</v>
+      </c>
+      <c r="AB114">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="AC114">
+        <v>0.81774193548387097</v>
+      </c>
+      <c r="AD114">
+        <v>0.87096774193548376</v>
+      </c>
+      <c r="AE114">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115">
+        <v>0.76975806451612905</v>
+      </c>
+      <c r="C115">
+        <v>0.76813172043010758</v>
+      </c>
+      <c r="D115">
+        <v>0.7714112903225806</v>
+      </c>
+      <c r="E115">
+        <v>0.78104838709677415</v>
+      </c>
+      <c r="F115">
+        <v>0.7577956989247312</v>
+      </c>
+      <c r="G115">
+        <v>0.77989247311827958</v>
+      </c>
+      <c r="H115">
+        <v>0.77775537634408598</v>
+      </c>
+      <c r="I115">
+        <v>0.77895161290322579</v>
+      </c>
+      <c r="K115" t="s">
+        <v>110</v>
+      </c>
+      <c r="L115">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="M115">
+        <v>0.25903225806451619</v>
+      </c>
+      <c r="N115">
+        <v>0.14725806451612911</v>
+      </c>
+      <c r="O115">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P115">
+        <v>0.44941820276497713</v>
+      </c>
+      <c r="Q115">
+        <v>0.7098540706605222</v>
+      </c>
+      <c r="R115">
+        <v>0.77775537634408598</v>
+      </c>
+      <c r="S115">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T115">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="U115">
+        <v>0.6769417849229501</v>
+      </c>
+      <c r="V115">
+        <v>0.70225044431933914</v>
+      </c>
+      <c r="W115">
+        <v>0.72100281284068302</v>
+      </c>
+      <c r="X115">
+        <v>0.44941820276497713</v>
+      </c>
+      <c r="Y115">
+        <v>0.62034399001536089</v>
+      </c>
+      <c r="Z115">
+        <v>0.64072502773510831</v>
+      </c>
+      <c r="AA115">
+        <v>0.6503511757401097</v>
+      </c>
+      <c r="AB115">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="AC115">
+        <v>0.82741935483870965</v>
+      </c>
+      <c r="AD115">
+        <v>0.86774193548387091</v>
+      </c>
+      <c r="AE115">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="C116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="D116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="E116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="F116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="G116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="H116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="I116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="K116" t="s">
+        <v>111</v>
+      </c>
+      <c r="L116">
+        <v>0.66129032258064513</v>
+      </c>
+      <c r="M116">
+        <v>0.26032258064516128</v>
+      </c>
+      <c r="N116">
+        <v>0.14838709677419351</v>
+      </c>
+      <c r="O116">
+        <v>1.6451612903225811E-2</v>
+      </c>
+      <c r="P116">
+        <v>0.44820852534562211</v>
+      </c>
+      <c r="Q116">
+        <v>0.71817012288786475</v>
+      </c>
+      <c r="R116">
+        <v>0.77895161290322579</v>
+      </c>
+      <c r="S116">
+        <v>0.83239247311827957</v>
+      </c>
+      <c r="T116">
+        <v>0.66129032258064513</v>
+      </c>
+      <c r="U116">
+        <v>0.68226776500892794</v>
+      </c>
+      <c r="V116">
+        <v>0.70517385335412308</v>
+      </c>
+      <c r="W116">
+        <v>0.72358625314130742</v>
+      </c>
+      <c r="X116">
+        <v>0.44820852534562211</v>
+      </c>
+      <c r="Y116">
+        <v>0.62366481054787504</v>
+      </c>
+      <c r="Z116">
+        <v>0.64238610013898023</v>
+      </c>
+      <c r="AA116">
+        <v>0.65218680465199008</v>
+      </c>
+      <c r="AB116">
+        <v>0.66129032258064513</v>
+      </c>
+      <c r="AC116">
+        <v>0.84193548387096784</v>
+      </c>
+      <c r="AD116">
+        <v>0.87096774193548376</v>
+      </c>
+      <c r="AE116">
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117">
+        <v>0.7</v>
+      </c>
+      <c r="C117">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="D117">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="E117">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="F117">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="G117">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="H117">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="I117">
+        <v>0.66129032258064513</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>10</v>
+      </c>
+      <c r="B118">
+        <v>0.67569639194713516</v>
+      </c>
+      <c r="C118">
+        <v>0.6671126897849724</v>
+      </c>
+      <c r="D118">
+        <v>0.6721386619249281</v>
+      </c>
+      <c r="E118">
+        <v>0.67340833792219734</v>
+      </c>
+      <c r="F118">
+        <v>0.66083863314591729</v>
+      </c>
+      <c r="G118">
+        <v>0.66991932689621814</v>
+      </c>
+      <c r="H118">
+        <v>0.6769417849229501</v>
+      </c>
+      <c r="I118">
+        <v>0.68226776500892794</v>
+      </c>
+    </row>
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>11</v>
+      </c>
+      <c r="B119">
+        <v>0.70512505515545087</v>
+      </c>
+      <c r="C119">
+        <v>0.69625897127709246</v>
+      </c>
+      <c r="D119">
+        <v>0.70245263163347793</v>
+      </c>
+      <c r="E119">
+        <v>0.70251917046246315</v>
+      </c>
+      <c r="F119">
+        <v>0.69255296422884216</v>
+      </c>
+      <c r="G119">
+        <v>0.70228681512738456</v>
+      </c>
+      <c r="H119">
+        <v>0.70225044431933914</v>
+      </c>
+      <c r="I119">
+        <v>0.70517385335412308</v>
+      </c>
+    </row>
+    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120">
+        <v>0.72665782150875668</v>
+      </c>
+      <c r="C120">
+        <v>0.71824283713922044</v>
+      </c>
+      <c r="D120">
+        <v>0.72267288339285729</v>
+      </c>
+      <c r="E120">
+        <v>0.71984080202643208</v>
+      </c>
+      <c r="F120">
+        <v>0.71720552563622242</v>
+      </c>
+      <c r="G120">
+        <v>0.72050050341331839</v>
+      </c>
+      <c r="H120">
+        <v>0.72100281284068302</v>
+      </c>
+      <c r="I120">
+        <v>0.72358625314130742</v>
+      </c>
+    </row>
+    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>13</v>
+      </c>
+      <c r="B121">
+        <v>0.46804723502304152</v>
+      </c>
+      <c r="C121">
+        <v>0.4527784178187404</v>
+      </c>
+      <c r="D121">
+        <v>0.45534562211981572</v>
+      </c>
+      <c r="E121">
+        <v>0.44365207373271892</v>
+      </c>
+      <c r="F121">
+        <v>0.45780529953917048</v>
+      </c>
+      <c r="G121">
+        <v>0.45048003072196618</v>
+      </c>
+      <c r="H121">
+        <v>0.44941820276497713</v>
+      </c>
+      <c r="I121">
+        <v>0.44820852534562211</v>
+      </c>
+    </row>
+    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>14</v>
+      </c>
+      <c r="B122">
+        <v>0.6246427611367128</v>
+      </c>
+      <c r="C122">
+        <v>0.61343362775217614</v>
+      </c>
+      <c r="D122">
+        <v>0.61857338069636447</v>
+      </c>
+      <c r="E122">
+        <v>0.61805619559651814</v>
+      </c>
+      <c r="F122">
+        <v>0.61012544802867386</v>
+      </c>
+      <c r="G122">
+        <v>0.61723790322580652</v>
+      </c>
+      <c r="H122">
+        <v>0.62034399001536089</v>
+      </c>
+      <c r="I122">
+        <v>0.62366481054787504</v>
+      </c>
+    </row>
+    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>15</v>
+      </c>
+      <c r="B123">
+        <v>0.64693134951113063</v>
+      </c>
+      <c r="C123">
+        <v>0.63604794973544976</v>
+      </c>
+      <c r="D123">
+        <v>0.64192677474215487</v>
+      </c>
+      <c r="E123">
+        <v>0.64041688001365427</v>
+      </c>
+      <c r="F123">
+        <v>0.63291546278009414</v>
+      </c>
+      <c r="G123">
+        <v>0.64048713822446535</v>
+      </c>
+      <c r="H123">
+        <v>0.64072502773510831</v>
+      </c>
+      <c r="I123">
+        <v>0.64238610013898023</v>
+      </c>
+    </row>
+    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>16</v>
+      </c>
+      <c r="B124">
+        <v>0.65739190523195057</v>
+      </c>
+      <c r="C124">
+        <v>0.64684139733675339</v>
+      </c>
+      <c r="D124">
+        <v>0.65182901437739937</v>
+      </c>
+      <c r="E124">
+        <v>0.64930170554740796</v>
+      </c>
+      <c r="F124">
+        <v>0.6446229701549766</v>
+      </c>
+      <c r="G124">
+        <v>0.64975592434607266</v>
+      </c>
+      <c r="H124">
+        <v>0.6503511757401097</v>
+      </c>
+      <c r="I124">
+        <v>0.65218680465199008</v>
+      </c>
+    </row>
+    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125">
+        <v>0.7</v>
+      </c>
+      <c r="C125">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="D125">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="E125">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="F125">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="G125">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="H125">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="I125">
+        <v>0.66129032258064513</v>
+      </c>
+    </row>
+    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>18</v>
+      </c>
+      <c r="B126">
+        <v>0.80806451612903218</v>
+      </c>
+      <c r="C126">
+        <v>0.81612903225806455</v>
+      </c>
+      <c r="D126">
+        <v>0.81935483870967762</v>
+      </c>
+      <c r="E126">
+        <v>0.82258064516129037</v>
+      </c>
+      <c r="F126">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="G126">
+        <v>0.81774193548387097</v>
+      </c>
+      <c r="H126">
+        <v>0.82741935483870965</v>
+      </c>
+      <c r="I126">
+        <v>0.84193548387096784</v>
+      </c>
+    </row>
+    <row r="127" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127">
+        <v>0.85967741935483866</v>
+      </c>
+      <c r="C127">
+        <v>0.85806451612903234</v>
+      </c>
+      <c r="D127">
+        <v>0.86290322580645162</v>
+      </c>
+      <c r="E127">
+        <v>0.87096774193548376</v>
+      </c>
+      <c r="F127">
+        <v>0.85483870967741937</v>
+      </c>
+      <c r="G127">
+        <v>0.87096774193548376</v>
+      </c>
+      <c r="H127">
+        <v>0.86774193548387091</v>
+      </c>
+      <c r="I127">
+        <v>0.87096774193548376</v>
+      </c>
+    </row>
+    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="C128">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="D128">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="E128">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="F128">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="G128">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="H128">
+        <v>0.88709677419354838</v>
+      </c>
+      <c r="I128">
+        <v>0.88709677419354838</v>
       </c>
     </row>
   </sheetData>
@@ -12056,20 +13897,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3A18D2-30FF-4570-A5C2-4E4FB86528D4}">
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.1640625" style="2"/>
+    <col min="1" max="1" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="25" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>87</v>
       </c>
@@ -12115,8 +13956,14 @@
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
       <c r="AC1" s="10"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="4" t="s">
         <v>83</v>
@@ -12202,8 +14049,20 @@
       <c r="AC2" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -12279,24 +14138,36 @@
       <c r="Y3" s="3">
         <v>1.2133333333329999E-4</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="Z3" s="3">
         <f>[3]Sheet1!B2</f>
         <v>0.33267326732673269</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="3">
         <f>[3]Sheet1!C2</f>
         <v>0.52475247524752477</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AB3" s="3">
         <f>[3]Sheet1!D2</f>
         <v>0.43433685881132428</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AC3" s="3">
         <f>[3]Sheet1!E2</f>
         <v>0.40422442244224421</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD3">
+        <v>0.7</v>
+      </c>
+      <c r="AE3">
+        <v>0.68967741935483873</v>
+      </c>
+      <c r="AF3">
+        <v>0.67569639194713516</v>
+      </c>
+      <c r="AG3">
+        <v>0.6246427611367128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
@@ -12372,24 +14243,36 @@
       <c r="Y4" s="8">
         <v>1.5333333333333E-3</v>
       </c>
-      <c r="Z4" s="12">
+      <c r="Z4" s="3">
         <f>[3]Sheet1!B3</f>
         <v>0.37227722772277227</v>
       </c>
-      <c r="AA4" s="12">
+      <c r="AA4" s="3">
         <f>[3]Sheet1!C3</f>
         <v>0.52871287128712874</v>
       </c>
-      <c r="AB4" s="12">
+      <c r="AB4" s="3">
         <f>[3]Sheet1!D3</f>
         <v>0.45956591316347828</v>
       </c>
-      <c r="AC4" s="12">
+      <c r="AC4" s="3">
         <f>[3]Sheet1!E3</f>
         <v>0.43623762376237629</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD4">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="AE4">
+        <v>0.69278225806451621</v>
+      </c>
+      <c r="AF4">
+        <v>0.66991932689621814</v>
+      </c>
+      <c r="AG4">
+        <v>0.61723790322580652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
@@ -12465,24 +14348,36 @@
       <c r="Y5" s="3">
         <v>5.7142857142857101E-5</v>
       </c>
-      <c r="Z5" s="12">
+      <c r="Z5" s="3">
         <f>[3]Sheet1!B4</f>
         <v>0.37029702970297029</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AA5" s="3">
         <f>[3]Sheet1!C4</f>
         <v>0.53861386138613865</v>
       </c>
-      <c r="AB5" s="12">
+      <c r="AB5" s="3">
         <f>[3]Sheet1!D4</f>
         <v>0.45923120656909389</v>
       </c>
-      <c r="AC5" s="12">
+      <c r="AC5" s="3">
         <f>[3]Sheet1!E4</f>
         <v>0.43280528052805273</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD5">
+        <v>0.67419354838709666</v>
+      </c>
+      <c r="AE5">
+        <v>0.67068548387096771</v>
+      </c>
+      <c r="AF5">
+        <v>0.66083863314591729</v>
+      </c>
+      <c r="AG5">
+        <v>0.61012544802867386</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
@@ -12574,8 +14469,20 @@
         <f>[3]Sheet1!E5</f>
         <v>0.46937293729372931</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD6">
+        <v>0.66612903225806452</v>
+      </c>
+      <c r="AE6">
+        <v>0.6897964669738863</v>
+      </c>
+      <c r="AF6">
+        <v>0.6671126897849724</v>
+      </c>
+      <c r="AG6">
+        <v>0.61343362775217614</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
@@ -12651,24 +14558,36 @@
       <c r="Y7" s="3">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="Z7" s="12">
+      <c r="Z7" s="3">
         <f>[3]Sheet1!B6</f>
         <v>0.40396039603960399</v>
       </c>
-      <c r="AA7" s="12">
+      <c r="AA7" s="3">
         <f>[3]Sheet1!C6</f>
         <v>0.55841584158415847</v>
       </c>
-      <c r="AB7" s="12">
+      <c r="AB7" s="3">
         <f>[3]Sheet1!D6</f>
         <v>0.48832212190279489</v>
       </c>
-      <c r="AC7" s="12">
+      <c r="AC7" s="3">
         <f>[3]Sheet1!E6</f>
         <v>0.46478547854785479</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD7">
+        <v>0.65645161290322585</v>
+      </c>
+      <c r="AE7">
+        <v>0.70302611367127488</v>
+      </c>
+      <c r="AF7">
+        <v>0.67340833792219734</v>
+      </c>
+      <c r="AG7">
+        <v>0.61805619559651814</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>71</v>
       </c>
@@ -12744,24 +14663,36 @@
       <c r="Y8" s="7">
         <v>2.2666666666666E-3</v>
       </c>
-      <c r="Z8" s="12">
+      <c r="Z8" s="3">
         <f>[3]Sheet1!B7</f>
         <v>0.39801980198019798</v>
       </c>
-      <c r="AA8" s="12">
+      <c r="AA8" s="3">
         <f>[3]Sheet1!C7</f>
         <v>0.55049504950495054</v>
       </c>
-      <c r="AB8" s="12">
+      <c r="AB8" s="3">
         <f>[3]Sheet1!D7</f>
         <v>0.47867078650248568</v>
       </c>
-      <c r="AC8" s="12">
+      <c r="AC8" s="3">
         <f>[3]Sheet1!E7</f>
         <v>0.45485148514851481</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD8">
+        <v>0.67096774193548381</v>
+      </c>
+      <c r="AE8">
+        <v>0.69269009216589861</v>
+      </c>
+      <c r="AF8">
+        <v>0.6721386619249281</v>
+      </c>
+      <c r="AG8">
+        <v>0.61857338069636447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -12837,24 +14768,36 @@
       <c r="Y9" s="3">
         <v>0</v>
       </c>
-      <c r="Z9" s="12">
+      <c r="Z9" s="3">
         <f>[3]Sheet1!B8</f>
         <v>0.39207920792079209</v>
       </c>
-      <c r="AA9" s="12">
+      <c r="AA9" s="3">
         <f>[3]Sheet1!C8</f>
         <v>0.56633663366336628</v>
       </c>
-      <c r="AB9" s="12">
+      <c r="AB9" s="3">
         <f>[3]Sheet1!D8</f>
         <v>0.4841750282211964</v>
       </c>
-      <c r="AC9" s="12">
+      <c r="AC9" s="3">
         <f>[3]Sheet1!E8</f>
         <v>0.45689768976897688</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD9">
+        <v>0.66451612903225799</v>
+      </c>
+      <c r="AE9">
+        <v>0.7098540706605222</v>
+      </c>
+      <c r="AF9">
+        <v>0.6769417849229501</v>
+      </c>
+      <c r="AG9">
+        <v>0.62034399001536089</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -12946,8 +14889,20 @@
         <f>[3]Sheet1!E9</f>
         <v>0.68306930693069312</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD10">
+        <v>0.66129032258064513</v>
+      </c>
+      <c r="AE10">
+        <v>0.71817012288786475</v>
+      </c>
+      <c r="AF10">
+        <v>0.68226776500892794</v>
+      </c>
+      <c r="AG10">
+        <v>0.62366481054787504</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -12974,7 +14929,8 @@
       <c r="Y11" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:Y1"/>

</xml_diff>

<commit_message>
update on results formatting
</commit_message>
<xml_diff>
--- a/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
+++ b/output/2015SB12/agg.pred.eval.mean.20.0.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farinam\PycharmProjects\LADy\output\2015SB12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75F6E8F-5EC4-4A12-B88C-5FA5CFB3D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CC4854-833A-4038-8555-4C0D5E1FC868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21210" windowHeight="12990" activeTab="2" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
+    <workbookView xWindow="11655" yWindow="2340" windowWidth="16110" windowHeight="12990" activeTab="2" xr2:uid="{4D2A36D4-8307-47D5-BCE7-FA144953644D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -518,20 +518,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6643,31 +6674,31 @@
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B156" s="12" t="s">
+      <c r="A156" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C156" s="12" t="s">
+      <c r="C156" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D156" s="12" t="s">
+      <c r="D156" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E156" s="12" t="s">
+      <c r="E156" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F156" s="12" t="s">
+      <c r="F156" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G156" s="12" t="s">
+      <c r="G156" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H156" s="12" t="s">
+      <c r="H156" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="I156" s="12" t="s">
+      <c r="I156" s="10" t="s">
         <v>103</v>
       </c>
     </row>
@@ -12715,31 +12746,31 @@
       </c>
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B108" s="12" t="s">
+      <c r="A108" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="12" t="s">
+      <c r="C108" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D108" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E108" s="12" t="s">
+      <c r="E108" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F108" s="12" t="s">
+      <c r="F108" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G108" s="12" t="s">
+      <c r="G108" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="H108" s="12" t="s">
+      <c r="H108" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="I108" s="12" t="s">
+      <c r="I108" s="10" t="s">
         <v>111</v>
       </c>
       <c r="K108" t="s">
@@ -13899,8 +13930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3A18D2-30FF-4570-A5C2-4E4FB86528D4}">
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AC15" sqref="AC15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AD10" sqref="AD10:AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13911,60 +13942,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10" t="s">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10" t="s">
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10" t="s">
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10" t="s">
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="4" t="s">
         <v>83</v>
       </c>
@@ -14154,16 +14185,16 @@
         <f>[3]Sheet1!E2</f>
         <v>0.40422442244224421</v>
       </c>
-      <c r="AD3">
+      <c r="AD3" s="7">
         <v>0.7</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="3">
         <v>0.68967741935483873</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="3">
         <v>0.67569639194713516</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="7">
         <v>0.6246427611367128</v>
       </c>
     </row>
@@ -14259,16 +14290,16 @@
         <f>[3]Sheet1!E3</f>
         <v>0.43623762376237629</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="3">
         <v>0.66612903225806452</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="3">
         <v>0.69278225806451621</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="3">
         <v>0.66991932689621814</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="3">
         <v>0.61723790322580652</v>
       </c>
     </row>
@@ -14364,16 +14395,16 @@
         <f>[3]Sheet1!E4</f>
         <v>0.43280528052805273</v>
       </c>
-      <c r="AD5">
+      <c r="AD5" s="8">
         <v>0.67419354838709666</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="3">
         <v>0.67068548387096771</v>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="3">
         <v>0.66083863314591729</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="3">
         <v>0.61012544802867386</v>
       </c>
     </row>
@@ -14469,16 +14500,16 @@
         <f>[3]Sheet1!E5</f>
         <v>0.46937293729372931</v>
       </c>
-      <c r="AD6">
+      <c r="AD6" s="13">
         <v>0.66612903225806452</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="13">
         <v>0.6897964669738863</v>
       </c>
-      <c r="AF6">
+      <c r="AF6" s="13">
         <v>0.6671126897849724</v>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="13">
         <v>0.61343362775217614</v>
       </c>
     </row>
@@ -14574,16 +14605,16 @@
         <f>[3]Sheet1!E6</f>
         <v>0.46478547854785479</v>
       </c>
-      <c r="AD7">
+      <c r="AD7" s="3">
         <v>0.65645161290322585</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="3">
         <v>0.70302611367127488</v>
       </c>
-      <c r="AF7">
+      <c r="AF7" s="3">
         <v>0.67340833792219734</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="3">
         <v>0.61805619559651814</v>
       </c>
     </row>
@@ -14679,16 +14710,16 @@
         <f>[3]Sheet1!E7</f>
         <v>0.45485148514851481</v>
       </c>
-      <c r="AD8">
+      <c r="AD8" s="3">
         <v>0.67096774193548381</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="3">
         <v>0.69269009216589861</v>
       </c>
-      <c r="AF8">
+      <c r="AF8" s="3">
         <v>0.6721386619249281</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="3">
         <v>0.61857338069636447</v>
       </c>
     </row>
@@ -14784,16 +14815,16 @@
         <f>[3]Sheet1!E8</f>
         <v>0.45689768976897688</v>
       </c>
-      <c r="AD9">
+      <c r="AD9" s="3">
         <v>0.66451612903225799</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="8">
         <v>0.7098540706605222</v>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="8">
         <v>0.6769417849229501</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="3">
         <v>0.62034399001536089</v>
       </c>
     </row>
@@ -14889,16 +14920,16 @@
         <f>[3]Sheet1!E9</f>
         <v>0.68306930693069312</v>
       </c>
-      <c r="AD10">
+      <c r="AD10" s="13">
         <v>0.66129032258064513</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="7">
         <v>0.71817012288786475</v>
       </c>
-      <c r="AF10">
+      <c r="AF10" s="7">
         <v>0.68226776500892794</v>
       </c>
-      <c r="AG10">
+      <c r="AG10" s="8">
         <v>0.62366481054787504</v>
       </c>
     </row>
@@ -14941,89 +14972,102 @@
     <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10">
+    <cfRule type="top10" dxfId="31" priority="32" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C10">
+    <cfRule type="top10" dxfId="30" priority="31" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10">
+    <cfRule type="top10" dxfId="29" priority="30" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E10">
+    <cfRule type="top10" dxfId="28" priority="29" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F10">
     <cfRule type="top10" dxfId="27" priority="28" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C10">
+  <conditionalFormatting sqref="G3:G10">
     <cfRule type="top10" dxfId="26" priority="27" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D10">
+  <conditionalFormatting sqref="H3:H10">
     <cfRule type="top10" dxfId="25" priority="26" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E10">
+  <conditionalFormatting sqref="I3:I10">
     <cfRule type="top10" dxfId="24" priority="25" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F10">
+  <conditionalFormatting sqref="J3:J10">
     <cfRule type="top10" dxfId="23" priority="24" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G10">
+  <conditionalFormatting sqref="K3:K10">
     <cfRule type="top10" dxfId="22" priority="23" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H10">
+  <conditionalFormatting sqref="L3:L10">
     <cfRule type="top10" dxfId="21" priority="22" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I10">
+  <conditionalFormatting sqref="M3:M10">
     <cfRule type="top10" dxfId="20" priority="21" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="N3:N10">
     <cfRule type="top10" dxfId="19" priority="20" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K10">
+  <conditionalFormatting sqref="O3:O10">
     <cfRule type="top10" dxfId="18" priority="19" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L10">
+  <conditionalFormatting sqref="P3:P10">
     <cfRule type="top10" dxfId="17" priority="18" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M10">
+  <conditionalFormatting sqref="Q3:Q10">
     <cfRule type="top10" dxfId="16" priority="17" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N10">
+  <conditionalFormatting sqref="R3:R10">
     <cfRule type="top10" dxfId="15" priority="16" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O10">
+  <conditionalFormatting sqref="S3:S10">
     <cfRule type="top10" dxfId="14" priority="15" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P10">
+  <conditionalFormatting sqref="T3:T10">
     <cfRule type="top10" dxfId="13" priority="14" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q10">
+  <conditionalFormatting sqref="U3:U10">
     <cfRule type="top10" dxfId="12" priority="13" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R10">
+  <conditionalFormatting sqref="V3:V10">
     <cfRule type="top10" dxfId="11" priority="12" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S10">
+  <conditionalFormatting sqref="W3:W10">
     <cfRule type="top10" dxfId="10" priority="11" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T10">
+  <conditionalFormatting sqref="X3:X10">
     <cfRule type="top10" dxfId="9" priority="10" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U10">
+  <conditionalFormatting sqref="Y3:Y10">
     <cfRule type="top10" dxfId="8" priority="9" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V10">
+  <conditionalFormatting sqref="Z3:Z10">
     <cfRule type="top10" dxfId="7" priority="8" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W10">
+  <conditionalFormatting sqref="AA3:AA10">
     <cfRule type="top10" dxfId="6" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X10">
+  <conditionalFormatting sqref="AB3:AB10">
     <cfRule type="top10" dxfId="5" priority="6" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y10">
+  <conditionalFormatting sqref="AC3:AC10">
     <cfRule type="top10" dxfId="4" priority="5" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:Z10">
+  <conditionalFormatting sqref="AD3:AD10">
     <cfRule type="top10" dxfId="3" priority="4" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA3:AA10">
+  <conditionalFormatting sqref="AE3:AE10">
     <cfRule type="top10" dxfId="2" priority="3" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB10">
+  <conditionalFormatting sqref="AF3:AF10">
     <cfRule type="top10" dxfId="1" priority="2" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC10">
+  <conditionalFormatting sqref="AG3:AG10">
     <cfRule type="top10" dxfId="0" priority="1" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>